<commit_message>
Changes to parsing and new data from dad
</commit_message>
<xml_diff>
--- a/monument_classes/grid refs.xlsx
+++ b/monument_classes/grid refs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/41e2a39a697455e7/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="503" documentId="8_{A4E60168-C7DA-486C-8F65-DF4D7C1E74F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8B84DE82-F9C7-47F9-BDF6-AF175DD7B489}"/>
+  <xr:revisionPtr revIDLastSave="586" documentId="8_{A4E60168-C7DA-486C-8F65-DF4D7C1E74F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E1E1DA83-3CE1-4E82-815B-4C1C2AF7A867}"/>
   <bookViews>
     <workbookView xWindow="-107" yWindow="-107" windowWidth="20847" windowHeight="11111" xr2:uid="{00C86CC1-D9DC-492E-B8C9-58A2E0E11513}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="435">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="458">
   <si>
     <t>Code number</t>
   </si>
@@ -153,9 +153,6 @@
     <t>Claughried, D&amp;G</t>
   </si>
   <si>
-    <t>Cnoc An Liath-Baihd , High</t>
-  </si>
-  <si>
     <t>Cockpit, C</t>
   </si>
   <si>
@@ -351,9 +348,6 @@
     <t>Lundin Links, Tay</t>
   </si>
   <si>
-    <t>Machrie Burn, Arran</t>
-  </si>
-  <si>
     <t>Machrie Moor 1, Arran</t>
   </si>
   <si>
@@ -540,9 +534,6 @@
     <t>Y Capel, Powys</t>
   </si>
   <si>
-    <t>Stonehenfe</t>
-  </si>
-  <si>
     <t>Castleruddsery</t>
   </si>
   <si>
@@ -565,9 +556,6 @@
   </si>
   <si>
     <t>NC893235</t>
-  </si>
-  <si>
-    <t>NC582049</t>
   </si>
   <si>
     <t>River Shin</t>
@@ -998,15 +986,9 @@
     <t>Leaze</t>
   </si>
   <si>
-    <t>N563262</t>
-  </si>
-  <si>
     <t>SX185799</t>
   </si>
   <si>
-    <t>NY576</t>
-  </si>
-  <si>
     <t>SH611217</t>
   </si>
   <si>
@@ -1356,13 +1338,100 @@
   </si>
   <si>
     <t>Airich</t>
+  </si>
+  <si>
+    <t>NO110311</t>
+  </si>
+  <si>
+    <t>NX919738</t>
+  </si>
+  <si>
+    <t>NX145625</t>
+  </si>
+  <si>
+    <t>SN130325</t>
+  </si>
+  <si>
+    <t>SD716158</t>
+  </si>
+  <si>
+    <t>Cnoc An Liath-Baihd ,</t>
+  </si>
+  <si>
+    <t>NY576375</t>
+  </si>
+  <si>
+    <t>NY563262</t>
+  </si>
+  <si>
+    <t>New Grnge</t>
+  </si>
+  <si>
+    <t>Aultan Broubster</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Balhomais </t>
+  </si>
+  <si>
+    <t>Barbrook 2</t>
+  </si>
+  <si>
+    <t>Boskednan,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bryn Y Gorlan </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cerrig Duon </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cnoc An Liath-Baihd </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lear Abele Hill </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Led Croen Yr Ych </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Llyn Y Tarw </t>
+  </si>
+  <si>
+    <t>Llyn Y Wrack,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mynydd Y Gelli </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sandy Road W </t>
+  </si>
+  <si>
+    <t>Stanton Drew</t>
+  </si>
+  <si>
+    <t>Threestone burn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wester Torrie </t>
+  </si>
+  <si>
+    <t>RECT</t>
+  </si>
+  <si>
+    <t>Stonehenge</t>
+  </si>
+  <si>
+    <t>C astleruddery</t>
+  </si>
+  <si>
+    <t>Shapbeck plantation</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="28" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1399,52 +1468,13 @@
     </font>
     <font>
       <sz val="28"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="28"/>
       <color rgb="FF494948"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="28"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="28"/>
-      <color rgb="FF333333"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="28"/>
-      <color rgb="FF000000"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="28"/>
       <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="28"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="26"/>
-      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -1455,40 +1485,7 @@
     </font>
     <font>
       <sz val="28"/>
-      <name val="Roboto"/>
-    </font>
-    <font>
-      <sz val="28"/>
       <color rgb="FF424242"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="28"/>
-      <color rgb="FF002020"/>
-      <name val="Verdana"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="24"/>
-      <color rgb="FF000000"/>
-      <name val="Roboto"/>
-    </font>
-    <font>
-      <sz val="24"/>
-      <color rgb="FF424241"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="24"/>
-      <color rgb="FF494948"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="24"/>
-      <color rgb="FF040809"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -1505,34 +1502,43 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="24"/>
-      <color theme="1"/>
-      <name val="Libre Baskerville"/>
-    </font>
-    <font>
-      <sz val="24"/>
-      <color rgb="FF002020"/>
-      <name val="Verdana"/>
+      <sz val="28"/>
+      <color rgb="FF424241"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="24"/>
+      <sz val="28"/>
+      <color rgb="FF040809"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="28"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="24"/>
-      <name val="Roboto"/>
+      <sz val="36"/>
+      <color rgb="FF494948"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
-      <sz val="24"/>
-      <color theme="1"/>
+      <sz val="28"/>
+      <color rgb="FF002020"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="28"/>
+      <color rgb="FF333333"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1547,19 +1553,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1577,7 +1577,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1585,79 +1585,46 @@
       <alignment textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1977,10 +1944,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6366B9E-07CC-4861-9D9F-9C4F681DA12F}">
-  <dimension ref="A1:E244"/>
+  <dimension ref="A1:E258"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" topLeftCell="A204" workbookViewId="0">
+      <selection activeCell="A258" sqref="A258"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="34.950000000000003" x14ac:dyDescent="0.65"/>
@@ -1994,82 +1961,82 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16"/>
+      <c r="B1" s="9"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
     </row>
     <row r="2" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A2" s="3"/>
-      <c r="B2" s="16"/>
+      <c r="B2" s="9"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
     </row>
     <row r="3" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A3" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>269</v>
+        <v>241</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>265</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
     </row>
     <row r="4" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A4" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="B4" s="41" t="s">
-        <v>403</v>
+        <v>242</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>397</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
     </row>
     <row r="5" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A5" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="B5" s="16" t="s">
-        <v>247</v>
+        <v>244</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>243</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
     </row>
     <row r="6" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A6" s="2" t="s">
-        <v>431</v>
-      </c>
-      <c r="B6" s="16" t="s">
-        <v>168</v>
+        <v>425</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>165</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
     </row>
     <row r="7" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A7" s="2" t="s">
-        <v>432</v>
-      </c>
-      <c r="B7" s="16" t="s">
-        <v>169</v>
+        <v>426</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>166</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A8" s="2" t="s">
-        <v>433</v>
-      </c>
-      <c r="B8" s="16" t="s">
-        <v>236</v>
+        <v>427</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>232</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A9" s="2" t="s">
-        <v>434</v>
-      </c>
-      <c r="B9" s="16" t="s">
-        <v>227</v>
+        <v>428</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>223</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -2078,8 +2045,8 @@
       <c r="A10" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="16" t="s">
-        <v>193</v>
+      <c r="B10" s="9" t="s">
+        <v>189</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -2088,8 +2055,8 @@
       <c r="A11" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="16" t="s">
-        <v>270</v>
+      <c r="B11" s="9" t="s">
+        <v>266</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
@@ -2098,8 +2065,8 @@
       <c r="A12" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B12" s="17" t="s">
-        <v>204</v>
+      <c r="B12" s="10" t="s">
+        <v>200</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -2108,18 +2075,18 @@
       <c r="A13" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B13" s="16" t="s">
-        <v>249</v>
+      <c r="B13" s="9" t="s">
+        <v>245</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A14" s="2" t="s">
-        <v>250</v>
-      </c>
-      <c r="B14" s="16" t="s">
-        <v>271</v>
+        <v>246</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>267</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -2128,18 +2095,18 @@
       <c r="A15" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B15" s="16" t="s">
-        <v>402</v>
+      <c r="B15" s="9" t="s">
+        <v>396</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A16" s="2" t="s">
-        <v>252</v>
-      </c>
-      <c r="B16" s="17" t="s">
-        <v>251</v>
+        <v>248</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>247</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -2148,8 +2115,8 @@
       <c r="A17" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B17" s="16" t="s">
-        <v>170</v>
+      <c r="B17" s="9" t="s">
+        <v>167</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
@@ -2158,8 +2125,8 @@
       <c r="A18" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B18" s="17" t="s">
-        <v>272</v>
+      <c r="B18" s="10" t="s">
+        <v>268</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
@@ -2168,8 +2135,8 @@
       <c r="A19" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B19" s="16" t="s">
-        <v>253</v>
+      <c r="B19" s="9" t="s">
+        <v>249</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
@@ -2178,8 +2145,8 @@
       <c r="A20" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B20" s="16" t="s">
-        <v>254</v>
+      <c r="B20" s="9" t="s">
+        <v>250</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
@@ -2188,8 +2155,8 @@
       <c r="A21" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B21" s="16" t="s">
-        <v>229</v>
+      <c r="B21" s="9" t="s">
+        <v>225</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
@@ -2198,18 +2165,18 @@
       <c r="A22" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B22" s="16" t="s">
-        <v>230</v>
+      <c r="B22" s="9" t="s">
+        <v>226</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
     </row>
     <row r="23" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
-      <c r="A23" s="2" t="s">
+      <c r="A23" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B23" s="17" t="s">
-        <v>255</v>
+      <c r="B23" s="18" t="s">
+        <v>251</v>
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
@@ -2218,8 +2185,8 @@
       <c r="A24" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B24" s="17" t="s">
-        <v>256</v>
+      <c r="B24" s="10" t="s">
+        <v>252</v>
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
@@ -2228,8 +2195,8 @@
       <c r="A25" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B25" s="16" t="s">
-        <v>257</v>
+      <c r="B25" s="9" t="s">
+        <v>253</v>
       </c>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
@@ -2238,8 +2205,8 @@
       <c r="A26" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B26" s="16" t="s">
-        <v>258</v>
+      <c r="B26" s="9" t="s">
+        <v>254</v>
       </c>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
@@ -2248,8 +2215,8 @@
       <c r="A27" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B27" s="16" t="s">
-        <v>413</v>
+      <c r="B27" s="9" t="s">
+        <v>407</v>
       </c>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
@@ -2258,8 +2225,8 @@
       <c r="A28" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B28" s="16" t="s">
-        <v>203</v>
+      <c r="B28" s="9" t="s">
+        <v>199</v>
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
@@ -2268,18 +2235,18 @@
       <c r="A29" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B29" s="16" t="s">
-        <v>259</v>
+      <c r="B29" s="9" t="s">
+        <v>255</v>
       </c>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
     </row>
     <row r="30" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A30" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="B30" s="16" t="s">
-        <v>260</v>
+        <v>224</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>256</v>
       </c>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
@@ -2288,8 +2255,8 @@
       <c r="A31" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B31" s="16" t="s">
-        <v>273</v>
+      <c r="B31" s="9" t="s">
+        <v>269</v>
       </c>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
@@ -2298,8 +2265,8 @@
       <c r="A32" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B32" s="16" t="s">
-        <v>261</v>
+      <c r="B32" s="9" t="s">
+        <v>257</v>
       </c>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
@@ -2308,8 +2275,8 @@
       <c r="A33" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B33" s="17" t="s">
-        <v>262</v>
+      <c r="B33" s="10" t="s">
+        <v>258</v>
       </c>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
@@ -2319,7 +2286,7 @@
         <v>22</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
@@ -2328,8 +2295,8 @@
       <c r="A35" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B35" s="16" t="s">
-        <v>263</v>
+      <c r="B35" s="9" t="s">
+        <v>259</v>
       </c>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
@@ -2338,8 +2305,8 @@
       <c r="A36" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B36" s="16" t="s">
-        <v>264</v>
+      <c r="B36" s="9" t="s">
+        <v>260</v>
       </c>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
@@ -2348,18 +2315,18 @@
       <c r="A37" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B37" s="16" t="s">
-        <v>265</v>
+      <c r="B37" s="9" t="s">
+        <v>261</v>
       </c>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
     </row>
     <row r="38" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A38" s="2" t="s">
-        <v>266</v>
-      </c>
-      <c r="B38" s="16" t="s">
-        <v>267</v>
+        <v>262</v>
+      </c>
+      <c r="B38" s="9" t="s">
+        <v>263</v>
       </c>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
@@ -2368,8 +2335,8 @@
       <c r="A39" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B39" s="15" t="s">
-        <v>212</v>
+      <c r="B39" s="8" t="s">
+        <v>208</v>
       </c>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
@@ -2378,18 +2345,18 @@
       <c r="A40" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B40" s="17" t="s">
-        <v>268</v>
+      <c r="B40" s="10" t="s">
+        <v>264</v>
       </c>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
     </row>
     <row r="41" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A41" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="B41" s="16" t="s">
-        <v>194</v>
+        <v>185</v>
+      </c>
+      <c r="B41" s="9" t="s">
+        <v>190</v>
       </c>
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
@@ -2399,7 +2366,7 @@
         <v>28</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>414</v>
+        <v>408</v>
       </c>
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
@@ -2409,7 +2376,7 @@
         <v>29</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
@@ -2419,7 +2386,7 @@
         <v>30</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
@@ -2428,18 +2395,18 @@
       <c r="A45" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B45" s="7" t="s">
-        <v>276</v>
+      <c r="B45" s="6" t="s">
+        <v>272</v>
       </c>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
     </row>
-    <row r="46" spans="1:4" ht="36" x14ac:dyDescent="0.75">
+    <row r="46" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A46" s="2" t="s">
         <v>32</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
@@ -2449,7 +2416,7 @@
         <v>33</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
@@ -2459,7 +2426,7 @@
         <v>34</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
@@ -2468,7 +2435,9 @@
       <c r="A49" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B49" s="4"/>
+      <c r="B49" s="2" t="s">
+        <v>433</v>
+      </c>
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
     </row>
@@ -2476,1506 +2445,1508 @@
       <c r="A50" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B50" s="14" t="s">
-        <v>279</v>
+      <c r="B50" s="7" t="s">
+        <v>275</v>
       </c>
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
     </row>
     <row r="51" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A51" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B51" s="6" t="s">
-        <v>171</v>
+        <v>434</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>168</v>
       </c>
       <c r="C51" s="1"/>
       <c r="D51" s="1"/>
     </row>
     <row r="52" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A52" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="C52" s="1"/>
       <c r="D52" s="1"/>
     </row>
-    <row r="53" spans="1:4" s="20" customFormat="1" ht="35.5" x14ac:dyDescent="0.7">
-      <c r="A53" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="B53" s="18"/>
-      <c r="C53" s="19"/>
-      <c r="D53" s="19"/>
+    <row r="53" spans="1:4" s="15" customFormat="1" ht="35.5" x14ac:dyDescent="0.7">
+      <c r="A53" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B53" s="9" t="s">
+        <v>429</v>
+      </c>
+      <c r="C53" s="14"/>
+      <c r="D53" s="14"/>
     </row>
     <row r="54" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A54" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="C54" s="1"/>
       <c r="D54" s="1"/>
     </row>
     <row r="55" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A55" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B55" s="21" t="s">
-        <v>281</v>
+        <v>40</v>
+      </c>
+      <c r="B55" s="10" t="s">
+        <v>277</v>
       </c>
       <c r="C55" s="1"/>
       <c r="D55" s="1"/>
     </row>
-    <row r="56" spans="1:4" ht="36" x14ac:dyDescent="0.75">
+    <row r="56" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A56" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B56" s="5" t="s">
-        <v>231</v>
+        <v>41</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>227</v>
       </c>
       <c r="C56" s="1"/>
       <c r="D56" s="1"/>
     </row>
     <row r="57" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A57" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B57" s="14" t="s">
-        <v>282</v>
+        <v>42</v>
+      </c>
+      <c r="B57" s="7" t="s">
+        <v>278</v>
       </c>
       <c r="C57" s="1"/>
       <c r="D57" s="1"/>
     </row>
     <row r="58" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A58" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B58" s="6" t="s">
-        <v>172</v>
+        <v>43</v>
+      </c>
+      <c r="B58" s="5" t="s">
+        <v>169</v>
       </c>
       <c r="C58" s="1"/>
       <c r="D58" s="1"/>
     </row>
     <row r="59" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A59" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B59" s="22" t="s">
-        <v>283</v>
+        <v>44</v>
+      </c>
+      <c r="B59" s="11" t="s">
+        <v>279</v>
       </c>
       <c r="C59" s="1"/>
       <c r="D59" s="1"/>
     </row>
     <row r="60" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A60" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C60" s="1"/>
       <c r="D60" s="1"/>
     </row>
     <row r="61" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A61" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="C61" s="1"/>
       <c r="D61" s="1"/>
     </row>
-    <row r="62" spans="1:4" ht="36" x14ac:dyDescent="0.75">
+    <row r="62" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A62" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="B62" s="5" t="s">
-        <v>232</v>
+        <v>229</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>228</v>
       </c>
       <c r="C62" s="1"/>
       <c r="D62" s="1"/>
     </row>
     <row r="63" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
-      <c r="A63" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B63" s="23" t="s">
-        <v>286</v>
+      <c r="A63" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B63" s="19" t="s">
+        <v>282</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="D63" s="1"/>
     </row>
     <row r="64" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A64" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="C64" s="1"/>
       <c r="D64" s="1"/>
     </row>
     <row r="65" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A65" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="C65" s="1"/>
       <c r="D65" s="1"/>
     </row>
-    <row r="66" spans="1:4" s="20" customFormat="1" ht="35.5" x14ac:dyDescent="0.7">
-      <c r="A66" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="B66" s="18"/>
-      <c r="C66" s="19"/>
-      <c r="D66" s="19"/>
+    <row r="66" spans="1:4" ht="44.6" x14ac:dyDescent="0.8">
+      <c r="A66" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="C66" s="16"/>
+      <c r="D66" s="1"/>
     </row>
     <row r="67" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A67" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="C67" s="1"/>
       <c r="D67" s="1"/>
     </row>
     <row r="68" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A68" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="C68" s="1"/>
       <c r="D68" s="1"/>
     </row>
     <row r="69" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A69" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="C69" s="1"/>
       <c r="D69" s="1"/>
     </row>
     <row r="70" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A70" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="C70" s="1"/>
       <c r="D70" s="1"/>
     </row>
-    <row r="71" spans="1:4" ht="36" x14ac:dyDescent="0.75">
+    <row r="71" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A71" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B71" s="5" t="s">
-        <v>234</v>
+        <v>55</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>230</v>
       </c>
       <c r="C71" s="1"/>
       <c r="D71" s="1"/>
     </row>
     <row r="72" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A72" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B72" s="24" t="s">
-        <v>292</v>
+        <v>56</v>
+      </c>
+      <c r="B72" s="13" t="s">
+        <v>288</v>
       </c>
       <c r="C72" s="1"/>
       <c r="D72" s="1"/>
     </row>
     <row r="73" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A73" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B73" s="6" t="s">
-        <v>198</v>
+        <v>57</v>
+      </c>
+      <c r="B73" s="5" t="s">
+        <v>194</v>
       </c>
       <c r="C73" s="1"/>
       <c r="D73" s="1"/>
     </row>
-    <row r="74" spans="1:4" ht="36" x14ac:dyDescent="0.75">
+    <row r="74" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A74" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B74" s="5" t="s">
-        <v>235</v>
+        <v>58</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>231</v>
       </c>
       <c r="C74" s="1"/>
       <c r="D74" s="1"/>
     </row>
     <row r="75" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A75" s="2" t="s">
-        <v>405</v>
+        <v>399</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>406</v>
+        <v>400</v>
       </c>
       <c r="C75" s="1"/>
       <c r="D75" s="1"/>
     </row>
     <row r="76" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A76" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>415</v>
+        <v>409</v>
       </c>
       <c r="C76" s="1"/>
       <c r="D76" s="1"/>
     </row>
-    <row r="77" spans="1:4" ht="36" x14ac:dyDescent="0.75">
+    <row r="77" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A77" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B77" s="8" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="C77" s="1"/>
       <c r="D77" s="1"/>
     </row>
     <row r="78" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A78" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="C78" s="1"/>
       <c r="D78" s="1"/>
     </row>
     <row r="79" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A79" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B79" s="25" t="s">
-        <v>294</v>
+        <v>62</v>
+      </c>
+      <c r="B79" s="17" t="s">
+        <v>290</v>
       </c>
       <c r="C79" s="1"/>
       <c r="D79" s="1"/>
     </row>
     <row r="80" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A80" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B80" s="26" t="s">
-        <v>295</v>
+        <v>63</v>
+      </c>
+      <c r="B80" s="7" t="s">
+        <v>291</v>
       </c>
       <c r="C80" s="1"/>
       <c r="D80" s="1"/>
     </row>
     <row r="81" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A81" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="B81" s="26" t="s">
-        <v>296</v>
+        <v>64</v>
+      </c>
+      <c r="B81" s="7" t="s">
+        <v>292</v>
       </c>
       <c r="C81" s="1"/>
       <c r="D81" s="1"/>
     </row>
-    <row r="82" spans="1:4" s="29" customFormat="1" ht="35.5" x14ac:dyDescent="0.7">
-      <c r="A82" s="27" t="s">
-        <v>66</v>
-      </c>
-      <c r="B82" s="27"/>
-      <c r="C82" s="28"/>
-      <c r="D82" s="28"/>
+    <row r="82" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+      <c r="A82" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>431</v>
+      </c>
+      <c r="C82" s="1"/>
+      <c r="D82" s="1"/>
     </row>
     <row r="83" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A83" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="C83" s="1"/>
       <c r="D83" s="1"/>
     </row>
     <row r="84" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A84" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="C84" s="1"/>
       <c r="D84" s="1"/>
     </row>
     <row r="85" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A85" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="C85" s="1"/>
       <c r="D85" s="1"/>
     </row>
     <row r="86" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A86" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="B86" s="6" t="s">
-        <v>173</v>
+        <v>69</v>
+      </c>
+      <c r="B86" s="5" t="s">
+        <v>170</v>
       </c>
       <c r="C86" s="1"/>
       <c r="D86" s="1"/>
     </row>
     <row r="87" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A87" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="C87" s="1"/>
       <c r="D87" s="1"/>
     </row>
-    <row r="88" spans="1:4" ht="36" x14ac:dyDescent="0.7">
+    <row r="88" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A88" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B88" s="9" t="s">
-        <v>215</v>
+        <v>71</v>
+      </c>
+      <c r="B88" s="5" t="s">
+        <v>211</v>
       </c>
       <c r="C88" s="1"/>
       <c r="D88" s="1"/>
     </row>
     <row r="89" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A89" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="C89" s="1"/>
       <c r="D89" s="1"/>
     </row>
     <row r="90" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A90" s="2" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C90" s="1"/>
       <c r="D90" s="1"/>
     </row>
     <row r="91" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A91" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="C91" s="1"/>
       <c r="D91" s="1"/>
     </row>
     <row r="92" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A92" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="C92" s="1"/>
       <c r="D92" s="1"/>
     </row>
     <row r="93" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A93" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>416</v>
+        <v>410</v>
       </c>
       <c r="C93" s="1"/>
       <c r="D93" s="1"/>
     </row>
     <row r="94" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A94" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="B94" s="30" t="s">
-        <v>303</v>
+        <v>76</v>
+      </c>
+      <c r="B94" s="12" t="s">
+        <v>299</v>
       </c>
       <c r="C94" s="1"/>
       <c r="D94" s="1"/>
     </row>
     <row r="95" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A95" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="B95" s="30" t="s">
-        <v>304</v>
+        <v>77</v>
+      </c>
+      <c r="B95" s="12" t="s">
+        <v>300</v>
       </c>
       <c r="C95" s="1"/>
       <c r="D95" s="1"/>
     </row>
     <row r="96" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A96" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="B96" s="30" t="s">
-        <v>305</v>
+        <v>78</v>
+      </c>
+      <c r="B96" s="12" t="s">
+        <v>301</v>
       </c>
       <c r="C96" s="1"/>
       <c r="D96" s="1"/>
     </row>
     <row r="97" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A97" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="B97" s="26" t="s">
-        <v>306</v>
+        <v>79</v>
+      </c>
+      <c r="B97" s="7" t="s">
+        <v>302</v>
       </c>
       <c r="C97" s="1"/>
       <c r="D97" s="1"/>
     </row>
     <row r="98" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A98" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="C98" s="1"/>
       <c r="D98" s="1"/>
     </row>
     <row r="99" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A99" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="C99" s="1"/>
       <c r="D99" s="1"/>
     </row>
-    <row r="100" spans="1:4" ht="36" x14ac:dyDescent="0.75">
+    <row r="100" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A100" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="B100" s="5" t="s">
-        <v>237</v>
+        <v>82</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>233</v>
       </c>
       <c r="C100" s="1"/>
       <c r="D100" s="1"/>
     </row>
     <row r="101" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A101" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="C101" s="1"/>
       <c r="D101" s="1"/>
     </row>
     <row r="102" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A102" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="C102" s="1"/>
       <c r="D102" s="1"/>
     </row>
     <row r="103" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A103" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="C103" s="1"/>
       <c r="D103" s="1"/>
     </row>
     <row r="104" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A104" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="C104" s="1"/>
       <c r="D104" s="1"/>
     </row>
     <row r="105" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A105" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="C105" s="1"/>
       <c r="D105" s="1"/>
     </row>
     <row r="106" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A106" s="2" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="C106" s="1"/>
       <c r="D106" s="1"/>
     </row>
     <row r="107" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A107" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="C107" s="1"/>
       <c r="D107" s="1"/>
     </row>
     <row r="108" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A108" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="B108" s="6" t="s">
-        <v>174</v>
+        <v>89</v>
+      </c>
+      <c r="B108" s="5" t="s">
+        <v>171</v>
       </c>
       <c r="C108" s="1"/>
       <c r="D108" s="1"/>
     </row>
     <row r="109" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A109" s="2" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="C109" s="1"/>
       <c r="D109" s="1"/>
     </row>
     <row r="110" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A110" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>315</v>
+        <v>436</v>
       </c>
       <c r="C110" s="1"/>
       <c r="D110" s="1"/>
     </row>
-    <row r="111" spans="1:4" ht="36" x14ac:dyDescent="0.75">
+    <row r="111" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A111" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B111" s="8" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="C111" s="1"/>
       <c r="D111" s="1"/>
     </row>
     <row r="112" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A112" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="C112" s="1"/>
       <c r="D112" s="1"/>
     </row>
-    <row r="113" spans="1:4" ht="36" x14ac:dyDescent="0.75">
+    <row r="113" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A113" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="B113" s="10" t="s">
-        <v>217</v>
+        <v>93</v>
+      </c>
+      <c r="B113" s="20" t="s">
+        <v>213</v>
       </c>
       <c r="C113" s="1"/>
       <c r="D113" s="1"/>
     </row>
-    <row r="114" spans="1:4" ht="36" x14ac:dyDescent="0.75">
+    <row r="114" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A114" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="B114" s="10" t="s">
-        <v>217</v>
+        <v>94</v>
+      </c>
+      <c r="B114" s="20" t="s">
+        <v>213</v>
       </c>
       <c r="C114" s="1"/>
       <c r="D114" s="1"/>
     </row>
     <row r="115" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A115" s="2" t="s">
-        <v>424</v>
+        <v>418</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>317</v>
+        <v>435</v>
       </c>
       <c r="C115" s="1"/>
       <c r="D115" s="1"/>
     </row>
     <row r="116" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A116" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
       <c r="C116" s="1"/>
       <c r="D116" s="1"/>
     </row>
-    <row r="117" spans="1:4" ht="36" x14ac:dyDescent="0.75">
+    <row r="117" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A117" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B117" s="10" t="s">
-        <v>219</v>
+        <v>96</v>
+      </c>
+      <c r="B117" s="20" t="s">
+        <v>215</v>
       </c>
       <c r="C117" s="1"/>
       <c r="D117" s="1"/>
     </row>
     <row r="118" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A118" s="2" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="C118" s="1"/>
       <c r="D118" s="1"/>
     </row>
     <row r="119" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A119" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="C119" s="1"/>
       <c r="D119" s="1"/>
     </row>
     <row r="120" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A120" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="B120" s="26" t="s">
-        <v>321</v>
+        <v>98</v>
+      </c>
+      <c r="B120" s="7" t="s">
+        <v>315</v>
       </c>
       <c r="C120" s="1"/>
       <c r="D120" s="1"/>
     </row>
     <row r="121" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A121" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="C121" s="1"/>
       <c r="D121" s="1"/>
     </row>
     <row r="122" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A122" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
       <c r="C122" s="1"/>
       <c r="D122" s="1"/>
     </row>
     <row r="123" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A123" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="B123" s="26" t="s">
-        <v>324</v>
+        <v>101</v>
+      </c>
+      <c r="B123" s="7" t="s">
+        <v>318</v>
       </c>
       <c r="C123" s="1"/>
       <c r="D123" s="1"/>
     </row>
-    <row r="124" spans="1:4" s="33" customFormat="1" ht="35.5" x14ac:dyDescent="0.7">
-      <c r="A124" s="31" t="s">
-        <v>103</v>
-      </c>
-      <c r="B124" s="31"/>
-      <c r="C124" s="32"/>
-      <c r="D124" s="32"/>
+    <row r="124" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+      <c r="A124" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B124" s="7" t="s">
+        <v>319</v>
+      </c>
+      <c r="C124" s="1"/>
+      <c r="D124" s="1"/>
     </row>
     <row r="125" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A125" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="B125" s="26" t="s">
-        <v>325</v>
+        <v>103</v>
+      </c>
+      <c r="B125" s="7" t="s">
+        <v>320</v>
       </c>
       <c r="C125" s="1"/>
       <c r="D125" s="1"/>
     </row>
     <row r="126" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A126" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="B126" s="26" t="s">
-        <v>326</v>
+        <v>104</v>
+      </c>
+      <c r="B126" s="7" t="s">
+        <v>321</v>
       </c>
       <c r="C126" s="1"/>
       <c r="D126" s="1"/>
     </row>
     <row r="127" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A127" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="B127" s="26" t="s">
-        <v>327</v>
+        <v>105</v>
+      </c>
+      <c r="B127" s="7" t="s">
+        <v>322</v>
       </c>
       <c r="C127" s="1"/>
       <c r="D127" s="1"/>
     </row>
     <row r="128" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A128" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="B128" s="26" t="s">
-        <v>328</v>
+        <v>105</v>
+      </c>
+      <c r="B128" s="7" t="s">
+        <v>323</v>
       </c>
       <c r="C128" s="1"/>
       <c r="D128" s="1"/>
     </row>
     <row r="129" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A129" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="B129" s="26" t="s">
-        <v>329</v>
+        <v>106</v>
+      </c>
+      <c r="B129" s="7" t="s">
+        <v>324</v>
       </c>
       <c r="C129" s="1"/>
       <c r="D129" s="1"/>
     </row>
     <row r="130" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A130" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="B130" s="26" t="s">
-        <v>330</v>
+        <v>107</v>
+      </c>
+      <c r="B130" s="2" t="s">
+        <v>234</v>
       </c>
       <c r="C130" s="1"/>
       <c r="D130" s="1"/>
     </row>
-    <row r="131" spans="1:4" ht="36" x14ac:dyDescent="0.75">
+    <row r="131" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A131" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="B131" s="5" t="s">
-        <v>238</v>
+        <v>108</v>
+      </c>
+      <c r="B131" s="10" t="s">
+        <v>325</v>
       </c>
       <c r="C131" s="1"/>
       <c r="D131" s="1"/>
     </row>
     <row r="132" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A132" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B132" s="26" t="s">
-        <v>331</v>
+        <v>109</v>
+      </c>
+      <c r="B132" s="5" t="s">
+        <v>216</v>
       </c>
       <c r="C132" s="1"/>
       <c r="D132" s="1"/>
     </row>
-    <row r="133" spans="1:4" ht="36" x14ac:dyDescent="0.7">
+    <row r="133" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A133" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="B133" s="9" t="s">
-        <v>220</v>
+        <v>110</v>
+      </c>
+      <c r="B133" s="5" t="s">
+        <v>326</v>
       </c>
       <c r="C133" s="1"/>
       <c r="D133" s="1"/>
     </row>
     <row r="134" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
-      <c r="A134" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="B134" s="34" t="s">
-        <v>332</v>
+      <c r="A134" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="B134" s="19" t="s">
+        <v>327</v>
       </c>
       <c r="C134" s="1"/>
       <c r="D134" s="1"/>
     </row>
     <row r="135" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A135" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="B135" s="35" t="s">
-        <v>333</v>
+        <v>112</v>
+      </c>
+      <c r="B135" s="2" t="s">
+        <v>328</v>
       </c>
       <c r="C135" s="1"/>
       <c r="D135" s="1"/>
     </row>
     <row r="136" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A136" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="B136" s="2" t="s">
-        <v>334</v>
+        <v>113</v>
+      </c>
+      <c r="B136" s="21" t="s">
+        <v>217</v>
       </c>
       <c r="C136" s="1"/>
       <c r="D136" s="1"/>
     </row>
     <row r="137" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A137" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="B137" s="11" t="s">
-        <v>221</v>
+        <v>114</v>
+      </c>
+      <c r="B137" s="2" t="s">
+        <v>329</v>
       </c>
       <c r="C137" s="1"/>
       <c r="D137" s="1"/>
     </row>
     <row r="138" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A138" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>335</v>
+        <v>235</v>
       </c>
       <c r="C138" s="1"/>
       <c r="D138" s="1"/>
     </row>
-    <row r="139" spans="1:4" ht="36" x14ac:dyDescent="0.75">
+    <row r="139" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A139" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="B139" s="5" t="s">
-        <v>239</v>
+        <v>116</v>
+      </c>
+      <c r="B139" s="2" t="s">
+        <v>330</v>
       </c>
       <c r="C139" s="1"/>
       <c r="D139" s="1"/>
     </row>
     <row r="140" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A140" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>336</v>
+        <v>236</v>
       </c>
       <c r="C140" s="1"/>
       <c r="D140" s="1"/>
     </row>
-    <row r="141" spans="1:4" ht="36" x14ac:dyDescent="0.75">
+    <row r="141" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A141" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="B141" s="5" t="s">
-        <v>240</v>
+        <v>118</v>
+      </c>
+      <c r="B141" s="2" t="s">
+        <v>218</v>
       </c>
       <c r="C141" s="1"/>
       <c r="D141" s="1"/>
     </row>
-    <row r="142" spans="1:4" ht="36" x14ac:dyDescent="0.75">
+    <row r="142" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A142" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="B142" s="5" t="s">
-        <v>222</v>
+        <v>119</v>
+      </c>
+      <c r="B142" s="2" t="s">
+        <v>331</v>
       </c>
       <c r="C142" s="1"/>
       <c r="D142" s="1"/>
     </row>
     <row r="143" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A143" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="B143" s="2" t="s">
-        <v>337</v>
+        <v>120</v>
+      </c>
+      <c r="B143" s="21" t="s">
+        <v>219</v>
       </c>
       <c r="C143" s="1"/>
       <c r="D143" s="1"/>
     </row>
     <row r="144" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A144" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="B144" s="11" t="s">
-        <v>223</v>
+        <v>121</v>
+      </c>
+      <c r="B144" s="21" t="s">
+        <v>332</v>
       </c>
       <c r="C144" s="1"/>
       <c r="D144" s="1"/>
     </row>
     <row r="145" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A145" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="B145" s="11" t="s">
-        <v>338</v>
+        <v>122</v>
+      </c>
+      <c r="B145" s="2" t="s">
+        <v>401</v>
       </c>
       <c r="C145" s="1"/>
       <c r="D145" s="1"/>
     </row>
     <row r="146" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A146" s="2" t="s">
-        <v>124</v>
+        <v>333</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>407</v>
+        <v>334</v>
       </c>
       <c r="C146" s="1"/>
       <c r="D146" s="1"/>
     </row>
     <row r="147" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A147" s="2" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="B147" s="2" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="C147" s="1"/>
       <c r="D147" s="1"/>
     </row>
     <row r="148" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A148" s="2" t="s">
-        <v>342</v>
+        <v>123</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="C148" s="1"/>
       <c r="D148" s="1"/>
     </row>
     <row r="149" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A149" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B149" s="2" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="C149" s="1"/>
       <c r="D149" s="1"/>
     </row>
     <row r="150" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A150" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="C150" s="1"/>
       <c r="D150" s="1"/>
     </row>
     <row r="151" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A151" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="C151" s="1"/>
       <c r="D151" s="1"/>
     </row>
     <row r="152" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A152" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B152" s="2" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="C152" s="1"/>
       <c r="D152" s="1"/>
     </row>
     <row r="153" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A153" s="2" t="s">
-        <v>129</v>
+        <v>344</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="C153" s="1"/>
       <c r="D153" s="1"/>
     </row>
     <row r="154" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A154" s="2" t="s">
-        <v>350</v>
+        <v>240</v>
       </c>
       <c r="B154" s="2" t="s">
-        <v>349</v>
+        <v>181</v>
       </c>
       <c r="C154" s="1"/>
       <c r="D154" s="1"/>
     </row>
     <row r="155" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A155" s="2" t="s">
-        <v>244</v>
-      </c>
-      <c r="B155" s="2" t="s">
-        <v>185</v>
+        <v>128</v>
+      </c>
+      <c r="B155" s="22" t="s">
+        <v>220</v>
       </c>
       <c r="C155" s="1"/>
       <c r="D155" s="1"/>
     </row>
-    <row r="156" spans="1:4" ht="36" x14ac:dyDescent="0.7">
+    <row r="156" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A156" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="B156" s="12" t="s">
-        <v>224</v>
+        <v>129</v>
+      </c>
+      <c r="B156" s="8" t="s">
+        <v>221</v>
       </c>
       <c r="C156" s="1"/>
       <c r="D156" s="1"/>
     </row>
-    <row r="157" spans="1:4" ht="36" x14ac:dyDescent="0.75">
+    <row r="157" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A157" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="B157" s="8" t="s">
-        <v>225</v>
+        <v>130</v>
+      </c>
+      <c r="B157" s="2" t="s">
+        <v>182</v>
       </c>
       <c r="C157" s="1"/>
       <c r="D157" s="1"/>
     </row>
     <row r="158" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A158" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B158" s="2" t="s">
-        <v>186</v>
+        <v>237</v>
       </c>
       <c r="C158" s="1"/>
       <c r="D158" s="1"/>
     </row>
-    <row r="159" spans="1:4" ht="36" x14ac:dyDescent="0.75">
+    <row r="159" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A159" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="B159" s="5" t="s">
-        <v>241</v>
+        <v>132</v>
+      </c>
+      <c r="B159" s="13" t="s">
+        <v>345</v>
       </c>
       <c r="C159" s="1"/>
       <c r="D159" s="1"/>
     </row>
     <row r="160" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A160" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="B160" s="36" t="s">
-        <v>351</v>
+        <v>346</v>
+      </c>
+      <c r="B160" s="2" t="s">
+        <v>347</v>
       </c>
       <c r="C160" s="1"/>
       <c r="D160" s="1"/>
     </row>
     <row r="161" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A161" s="2" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="B161" s="2" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="C161" s="1"/>
       <c r="D161" s="1"/>
     </row>
     <row r="162" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A162" s="2" t="s">
-        <v>355</v>
-      </c>
-      <c r="B162" s="2" t="s">
-        <v>354</v>
+        <v>133</v>
+      </c>
+      <c r="B162" s="7" t="s">
+        <v>350</v>
       </c>
       <c r="C162" s="1"/>
       <c r="D162" s="1"/>
     </row>
     <row r="163" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A163" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="B163" s="26" t="s">
-        <v>356</v>
+        <v>134</v>
+      </c>
+      <c r="B163" s="7" t="s">
+        <v>351</v>
       </c>
       <c r="C163" s="1"/>
       <c r="D163" s="1"/>
     </row>
     <row r="164" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A164" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="B164" s="26" t="s">
-        <v>357</v>
+        <v>135</v>
+      </c>
+      <c r="B164" s="2" t="s">
+        <v>197</v>
       </c>
       <c r="C164" s="1"/>
       <c r="D164" s="1"/>
     </row>
     <row r="165" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A165" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B165" s="2" t="s">
-        <v>201</v>
+        <v>352</v>
       </c>
       <c r="C165" s="1"/>
       <c r="D165" s="1"/>
     </row>
     <row r="166" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A166" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="B166" s="1" t="s">
-        <v>358</v>
+        <v>137</v>
+      </c>
+      <c r="B166" s="2" t="s">
+        <v>353</v>
       </c>
       <c r="C166" s="1"/>
       <c r="D166" s="1"/>
     </row>
     <row r="167" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A167" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B167" s="2" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
       <c r="C167" s="1"/>
       <c r="D167" s="1"/>
     </row>
     <row r="168" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A168" s="2" t="s">
-        <v>140</v>
+        <v>355</v>
       </c>
       <c r="B168" s="2" t="s">
-        <v>360</v>
+        <v>202</v>
       </c>
       <c r="C168" s="1"/>
       <c r="D168" s="1"/>
     </row>
     <row r="169" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A169" s="2" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="B169" s="2" t="s">
-        <v>206</v>
+        <v>356</v>
       </c>
       <c r="C169" s="1"/>
       <c r="D169" s="1"/>
     </row>
     <row r="170" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A170" s="2" t="s">
-        <v>363</v>
-      </c>
-      <c r="B170" s="2" t="s">
-        <v>362</v>
+        <v>358</v>
+      </c>
+      <c r="B170" s="10" t="s">
+        <v>359</v>
       </c>
       <c r="C170" s="1"/>
       <c r="D170" s="1"/>
     </row>
     <row r="171" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A171" s="2" t="s">
-        <v>364</v>
-      </c>
-      <c r="B171" s="37" t="s">
-        <v>365</v>
+        <v>139</v>
+      </c>
+      <c r="B171" s="2" t="s">
+        <v>360</v>
       </c>
       <c r="C171" s="1"/>
       <c r="D171" s="1"/>
     </row>
     <row r="172" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A172" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="B172" s="2" t="s">
-        <v>366</v>
+        <v>140</v>
+      </c>
+      <c r="B172" s="13" t="s">
+        <v>361</v>
       </c>
       <c r="C172" s="1"/>
       <c r="D172" s="1"/>
     </row>
     <row r="173" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A173" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="B173" s="36" t="s">
-        <v>367</v>
+        <v>141</v>
+      </c>
+      <c r="B173" s="13" t="s">
+        <v>362</v>
       </c>
       <c r="C173" s="1"/>
       <c r="D173" s="1"/>
     </row>
     <row r="174" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A174" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="B174" s="36" t="s">
-        <v>368</v>
+        <v>142</v>
+      </c>
+      <c r="B174" s="2" t="s">
+        <v>363</v>
       </c>
       <c r="C174" s="1"/>
       <c r="D174" s="1"/>
     </row>
     <row r="175" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A175" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B175" s="2" t="s">
-        <v>369</v>
+        <v>364</v>
       </c>
       <c r="C175" s="1"/>
       <c r="D175" s="1"/>
     </row>
     <row r="176" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A176" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B176" s="2" t="s">
-        <v>370</v>
+        <v>365</v>
       </c>
       <c r="C176" s="1"/>
       <c r="D176" s="1"/>
     </row>
     <row r="177" spans="1:5" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A177" s="2" t="s">
-        <v>146</v>
+        <v>367</v>
       </c>
       <c r="B177" s="2" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
       <c r="C177" s="1"/>
       <c r="D177" s="1"/>
     </row>
     <row r="178" spans="1:5" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A178" s="2" t="s">
-        <v>373</v>
-      </c>
-      <c r="B178" s="2" t="s">
-        <v>372</v>
+        <v>145</v>
+      </c>
+      <c r="B178" s="5" t="s">
+        <v>175</v>
       </c>
       <c r="C178" s="1"/>
       <c r="D178" s="1"/>
     </row>
     <row r="179" spans="1:5" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A179" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="B179" s="6" t="s">
-        <v>179</v>
+        <v>369</v>
+      </c>
+      <c r="B179" s="2" t="s">
+        <v>368</v>
       </c>
       <c r="C179" s="1"/>
       <c r="D179" s="1"/>
     </row>
     <row r="180" spans="1:5" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A180" s="2" t="s">
-        <v>375</v>
+        <v>146</v>
       </c>
       <c r="B180" s="2" t="s">
-        <v>374</v>
+        <v>411</v>
       </c>
       <c r="C180" s="1"/>
       <c r="D180" s="1"/>
     </row>
     <row r="181" spans="1:5" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A181" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B181" s="2" t="s">
-        <v>417</v>
+        <v>238</v>
       </c>
       <c r="C181" s="1"/>
       <c r="D181" s="1"/>
     </row>
-    <row r="182" spans="1:5" ht="36" x14ac:dyDescent="0.75">
+    <row r="182" spans="1:5" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A182" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="B182" s="5" t="s">
-        <v>242</v>
+        <v>148</v>
+      </c>
+      <c r="B182" s="2" t="s">
+        <v>370</v>
       </c>
       <c r="C182" s="1"/>
       <c r="D182" s="1"/>
     </row>
     <row r="183" spans="1:5" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A183" s="2" t="s">
-        <v>150</v>
+        <v>372</v>
       </c>
       <c r="B183" s="2" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="C183" s="1"/>
       <c r="D183" s="1"/>
     </row>
     <row r="184" spans="1:5" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A184" s="2" t="s">
-        <v>378</v>
-      </c>
-      <c r="B184" s="1" t="s">
-        <v>377</v>
+        <v>149</v>
+      </c>
+      <c r="B184" s="2" t="s">
+        <v>374</v>
       </c>
       <c r="C184" s="1"/>
       <c r="D184" s="1"/>
     </row>
     <row r="185" spans="1:5" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A185" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="B185" s="2" t="s">
-        <v>380</v>
+        <v>150</v>
+      </c>
+      <c r="B185" s="5" t="s">
+        <v>373</v>
       </c>
       <c r="C185" s="1"/>
       <c r="D185" s="1"/>
     </row>
     <row r="186" spans="1:5" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A186" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="B186" s="38" t="s">
-        <v>379</v>
+        <v>151</v>
+      </c>
+      <c r="B186" s="21" t="s">
+        <v>375</v>
       </c>
       <c r="C186" s="1"/>
       <c r="D186" s="1"/>
     </row>
     <row r="187" spans="1:5" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A187" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="B187" s="39" t="s">
-        <v>381</v>
+        <v>377</v>
+      </c>
+      <c r="B187" s="2" t="s">
+        <v>376</v>
       </c>
       <c r="C187" s="1"/>
       <c r="D187" s="1"/>
+      <c r="E187">
+        <v>592</v>
+      </c>
     </row>
     <row r="188" spans="1:5" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A188" s="2" t="s">
-        <v>383</v>
-      </c>
-      <c r="B188" s="2" t="s">
-        <v>382</v>
+        <v>152</v>
+      </c>
+      <c r="B188" s="7" t="s">
+        <v>378</v>
       </c>
       <c r="C188" s="1"/>
       <c r="D188" s="1"/>
-      <c r="E188">
-        <v>592</v>
-      </c>
     </row>
     <row r="189" spans="1:5" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A189" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="B189" s="26" t="s">
-        <v>384</v>
+        <v>153</v>
+      </c>
+      <c r="B189" s="5" t="s">
+        <v>198</v>
       </c>
       <c r="C189" s="1"/>
       <c r="D189" s="1"/>
     </row>
     <row r="190" spans="1:5" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A190" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="B190" s="6" t="s">
-        <v>202</v>
+        <v>154</v>
+      </c>
+      <c r="B190" s="2" t="s">
+        <v>379</v>
       </c>
       <c r="C190" s="1"/>
       <c r="D190" s="1"/>
     </row>
     <row r="191" spans="1:5" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A191" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B191" s="2" t="s">
-        <v>385</v>
+        <v>239</v>
       </c>
       <c r="C191" s="1"/>
       <c r="D191" s="1"/>
     </row>
-    <row r="192" spans="1:5" ht="36" x14ac:dyDescent="0.75">
+    <row r="192" spans="1:5" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A192" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="B192" s="5" t="s">
-        <v>243</v>
+        <v>156</v>
+      </c>
+      <c r="B192" s="2" t="s">
+        <v>286</v>
       </c>
       <c r="C192" s="1"/>
       <c r="D192" s="1"/>
     </row>
     <row r="193" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A193" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="B193" s="2" t="s">
-        <v>290</v>
+        <v>157</v>
+      </c>
+      <c r="B193" s="7" t="s">
+        <v>380</v>
       </c>
       <c r="C193" s="1"/>
       <c r="D193" s="1"/>
     </row>
     <row r="194" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A194" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="B194" s="26" t="s">
-        <v>386</v>
+        <v>158</v>
+      </c>
+      <c r="B194" s="2" t="s">
+        <v>381</v>
       </c>
       <c r="C194" s="1"/>
       <c r="D194" s="1"/>
     </row>
     <row r="195" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A195" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B195" s="2" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="C195" s="1"/>
       <c r="D195" s="1"/>
     </row>
     <row r="196" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A196" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B196" s="2" t="s">
-        <v>389</v>
+        <v>382</v>
       </c>
       <c r="C196" s="1"/>
       <c r="D196" s="1"/>
     </row>
     <row r="197" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A197" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="B197" s="2" t="s">
-        <v>388</v>
+        <v>161</v>
+      </c>
+      <c r="B197" s="5" t="s">
+        <v>184</v>
       </c>
       <c r="C197" s="1"/>
       <c r="D197" s="1"/>
     </row>
     <row r="198" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A198" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="B198" s="6" t="s">
-        <v>188</v>
+        <v>162</v>
+      </c>
+      <c r="B198" s="2" t="s">
+        <v>384</v>
       </c>
       <c r="C198" s="1"/>
       <c r="D198" s="1"/>
     </row>
     <row r="199" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A199" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="B199" s="2" t="s">
-        <v>390</v>
+        <v>163</v>
+      </c>
+      <c r="B199" s="8" t="s">
+        <v>222</v>
       </c>
       <c r="C199" s="1"/>
       <c r="D199" s="1"/>
     </row>
-    <row r="200" spans="1:4" ht="36" x14ac:dyDescent="0.75">
-      <c r="A200" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="B200" s="8" t="s">
-        <v>226</v>
-      </c>
+    <row r="200" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="C200" s="1"/>
       <c r="D200" s="1"/>
     </row>
@@ -3984,199 +3955,210 @@
       <c r="D201" s="1"/>
     </row>
     <row r="202" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+      <c r="A202" s="23" t="s">
+        <v>340</v>
+      </c>
+      <c r="B202" s="2" t="s">
+        <v>387</v>
+      </c>
       <c r="C202" s="1"/>
       <c r="D202" s="1"/>
     </row>
     <row r="203" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
       <c r="A203" s="2" t="s">
-        <v>346</v>
+        <v>207</v>
       </c>
       <c r="B203" s="2" t="s">
-        <v>393</v>
-      </c>
-      <c r="C203" s="1"/>
+        <v>432</v>
+      </c>
+      <c r="C203" s="1" t="s">
+        <v>454</v>
+      </c>
       <c r="D203" s="1"/>
     </row>
     <row r="204" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
-      <c r="A204" s="40" t="s">
-        <v>211</v>
+      <c r="A204" s="23" t="s">
+        <v>186</v>
+      </c>
+      <c r="B204" s="6" t="s">
+        <v>187</v>
       </c>
       <c r="C204" s="1"/>
       <c r="D204" s="1"/>
     </row>
     <row r="205" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
-      <c r="A205" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="B205" s="7" t="s">
-        <v>191</v>
+      <c r="A205" s="23" t="s">
+        <v>164</v>
+      </c>
+      <c r="B205" s="4" t="s">
+        <v>388</v>
       </c>
       <c r="C205" s="1"/>
       <c r="D205" s="1"/>
     </row>
     <row r="206" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
-      <c r="A206" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="B206" s="4" t="s">
-        <v>394</v>
+      <c r="A206" s="23" t="s">
+        <v>173</v>
+      </c>
+      <c r="B206" s="2" t="s">
+        <v>174</v>
       </c>
       <c r="C206" s="1"/>
       <c r="D206" s="1"/>
     </row>
     <row r="207" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
-      <c r="A207" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="B207" s="13" t="s">
-        <v>178</v>
+      <c r="A207" s="23" t="s">
+        <v>385</v>
+      </c>
+      <c r="B207" s="4" t="s">
+        <v>389</v>
       </c>
       <c r="C207" s="1"/>
       <c r="D207" s="1"/>
     </row>
     <row r="208" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
-      <c r="A208" s="2" t="s">
-        <v>391</v>
+      <c r="A208" s="23" t="s">
+        <v>205</v>
       </c>
       <c r="B208" s="2" t="s">
-        <v>395</v>
+        <v>206</v>
       </c>
       <c r="C208" s="1"/>
       <c r="D208" s="1"/>
     </row>
     <row r="209" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
-      <c r="A209" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="B209" s="2" t="s">
-        <v>210</v>
+      <c r="A209" s="23" t="s">
+        <v>179</v>
+      </c>
+      <c r="B209" s="5" t="s">
+        <v>180</v>
       </c>
       <c r="C209" s="1"/>
       <c r="D209" s="1"/>
     </row>
     <row r="210" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
-      <c r="A210" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="B210" s="6" t="s">
-        <v>184</v>
+      <c r="A210" s="23" t="s">
+        <v>386</v>
+      </c>
+      <c r="B210" s="10" t="s">
+        <v>390</v>
       </c>
       <c r="C210" s="1"/>
       <c r="D210" s="1"/>
     </row>
     <row r="211" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
-      <c r="A211" s="2" t="s">
-        <v>392</v>
-      </c>
-      <c r="B211" s="14" t="s">
-        <v>396</v>
+      <c r="A211" s="23" t="s">
+        <v>455</v>
+      </c>
+      <c r="B211" s="2" t="s">
+        <v>391</v>
       </c>
       <c r="C211" s="1"/>
       <c r="D211" s="1"/>
     </row>
     <row r="212" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
-      <c r="A212" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="B212" s="6" t="s">
-        <v>175</v>
+      <c r="A212" s="23" t="s">
+        <v>392</v>
+      </c>
+      <c r="B212" s="10" t="s">
+        <v>394</v>
       </c>
       <c r="C212" s="1"/>
       <c r="D212" s="1"/>
     </row>
     <row r="213" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
-      <c r="A213" s="2" t="s">
-        <v>166</v>
+      <c r="A213" s="23" t="s">
+        <v>395</v>
       </c>
       <c r="B213" s="2" t="s">
-        <v>397</v>
+        <v>191</v>
       </c>
       <c r="C213" s="1"/>
       <c r="D213" s="1"/>
     </row>
     <row r="214" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
-      <c r="A214" s="2" t="s">
-        <v>398</v>
-      </c>
-      <c r="B214" s="26" t="s">
-        <v>400</v>
+      <c r="A214" s="23" t="s">
+        <v>403</v>
+      </c>
+      <c r="B214" s="2" t="s">
+        <v>404</v>
       </c>
       <c r="C214" s="1"/>
       <c r="D214" s="1"/>
     </row>
     <row r="215" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
-      <c r="A215" s="2" t="s">
-        <v>401</v>
+      <c r="A215" s="23" t="s">
+        <v>183</v>
       </c>
       <c r="B215" s="2" t="s">
-        <v>195</v>
+        <v>405</v>
       </c>
       <c r="C215" s="1"/>
       <c r="D215" s="1"/>
     </row>
     <row r="216" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
-      <c r="A216" s="2" t="s">
-        <v>409</v>
-      </c>
-      <c r="B216" s="2" t="s">
-        <v>410</v>
+      <c r="A216" s="23" t="s">
+        <v>406</v>
+      </c>
+      <c r="B216" s="10" t="s">
+        <v>188</v>
       </c>
       <c r="C216" s="1"/>
       <c r="D216" s="1"/>
     </row>
     <row r="217" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
-      <c r="A217" s="2" t="s">
-        <v>187</v>
+      <c r="A217" s="23" t="s">
+        <v>393</v>
       </c>
       <c r="B217" s="2" t="s">
-        <v>411</v>
+        <v>402</v>
       </c>
       <c r="C217" s="1"/>
       <c r="D217" s="1"/>
     </row>
     <row r="218" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
-      <c r="A218" s="2" t="s">
-        <v>412</v>
-      </c>
-      <c r="B218" s="14" t="s">
-        <v>192</v>
+      <c r="A218" s="23" t="s">
+        <v>195</v>
+      </c>
+      <c r="B218" s="2" t="s">
+        <v>196</v>
       </c>
       <c r="C218" s="1"/>
       <c r="D218" s="1"/>
     </row>
     <row r="219" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
-      <c r="A219" s="2" t="s">
-        <v>399</v>
+      <c r="A219" s="23" t="s">
+        <v>413</v>
       </c>
       <c r="B219" s="2" t="s">
-        <v>408</v>
+        <v>412</v>
       </c>
       <c r="C219" s="1"/>
       <c r="D219" s="1"/>
     </row>
     <row r="220" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
-      <c r="A220" s="2" t="s">
-        <v>199</v>
+      <c r="A220" s="23" t="s">
+        <v>414</v>
       </c>
       <c r="B220" s="2" t="s">
-        <v>200</v>
+        <v>416</v>
       </c>
       <c r="C220" s="1"/>
       <c r="D220" s="1"/>
     </row>
     <row r="221" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
-      <c r="A221" s="2" t="s">
-        <v>419</v>
+      <c r="A221" s="23" t="s">
+        <v>415</v>
       </c>
       <c r="B221" s="2" t="s">
-        <v>418</v>
-      </c>
-      <c r="C221" s="1"/>
+        <v>417</v>
+      </c>
+      <c r="C221" s="2"/>
       <c r="D221" s="1"/>
     </row>
     <row r="222" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
-      <c r="A222" s="2" t="s">
-        <v>420</v>
+      <c r="A222" s="23" t="s">
+        <v>421</v>
       </c>
       <c r="B222" s="2" t="s">
         <v>422</v>
@@ -4185,120 +4167,232 @@
       <c r="D222" s="1"/>
     </row>
     <row r="223" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
-      <c r="A223" s="2" t="s">
-        <v>421</v>
+      <c r="A223" s="23" t="s">
+        <v>419</v>
       </c>
       <c r="B223" s="2" t="s">
         <v>423</v>
       </c>
-      <c r="C223" s="2"/>
+      <c r="C223" s="1"/>
       <c r="D223" s="1"/>
     </row>
     <row r="224" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
-      <c r="A224" s="2" t="s">
-        <v>427</v>
+      <c r="A224" s="23" t="s">
+        <v>420</v>
       </c>
       <c r="B224" s="2" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="C224" s="1"/>
       <c r="D224" s="1"/>
     </row>
     <row r="225" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
-      <c r="A225" s="2" t="s">
-        <v>425</v>
-      </c>
-      <c r="B225" s="2" t="s">
-        <v>429</v>
-      </c>
+      <c r="A225" s="4" t="s">
+        <v>437</v>
+      </c>
+      <c r="B225" s="4"/>
       <c r="C225" s="1"/>
       <c r="D225" s="1"/>
     </row>
     <row r="226" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
-      <c r="A226" s="2" t="s">
-        <v>426</v>
-      </c>
-      <c r="B226" s="2" t="s">
-        <v>430</v>
-      </c>
       <c r="C226" s="1"/>
       <c r="D226" s="1"/>
     </row>
     <row r="227" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+      <c r="A227" s="23" t="s">
+        <v>438</v>
+      </c>
       <c r="C227" s="1"/>
       <c r="D227" s="1"/>
     </row>
     <row r="228" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+      <c r="A228" s="23" t="s">
+        <v>439</v>
+      </c>
       <c r="C228" s="1"/>
       <c r="D228" s="1"/>
     </row>
     <row r="229" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+      <c r="A229" s="23" t="s">
+        <v>440</v>
+      </c>
       <c r="C229" s="1"/>
       <c r="D229" s="1"/>
     </row>
     <row r="230" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+      <c r="A230" s="23" t="s">
+        <v>441</v>
+      </c>
       <c r="C230" s="1"/>
       <c r="D230" s="1"/>
     </row>
     <row r="231" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+      <c r="A231" s="23" t="s">
+        <v>442</v>
+      </c>
       <c r="C231" s="1"/>
       <c r="D231" s="1"/>
     </row>
     <row r="232" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+      <c r="A232" s="23" t="s">
+        <v>393</v>
+      </c>
       <c r="C232" s="1"/>
       <c r="D232" s="1"/>
     </row>
     <row r="233" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+      <c r="A233" s="23" t="s">
+        <v>456</v>
+      </c>
       <c r="C233" s="1"/>
       <c r="D233" s="1"/>
     </row>
     <row r="234" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+      <c r="A234" s="23" t="s">
+        <v>443</v>
+      </c>
       <c r="C234" s="1"/>
       <c r="D234" s="1"/>
     </row>
     <row r="235" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+      <c r="A235" s="23" t="s">
+        <v>444</v>
+      </c>
       <c r="C235" s="1"/>
       <c r="D235" s="1"/>
     </row>
     <row r="236" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+      <c r="A236" s="23" t="s">
+        <v>229</v>
+      </c>
       <c r="C236" s="1"/>
       <c r="D236" s="1"/>
     </row>
     <row r="237" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+      <c r="A237" s="23" t="s">
+        <v>399</v>
+      </c>
       <c r="C237" s="1"/>
       <c r="D237" s="1"/>
     </row>
     <row r="238" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+      <c r="A238" s="23" t="s">
+        <v>415</v>
+      </c>
       <c r="C238" s="1"/>
       <c r="D238" s="1"/>
     </row>
     <row r="239" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+      <c r="A239" s="23" t="s">
+        <v>445</v>
+      </c>
       <c r="C239" s="1"/>
       <c r="D239" s="1"/>
     </row>
     <row r="240" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+      <c r="A240" s="23" t="s">
+        <v>310</v>
+      </c>
       <c r="C240" s="1"/>
       <c r="D240" s="1"/>
     </row>
-    <row r="241" spans="3:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row r="241" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+      <c r="A241" s="23" t="s">
+        <v>446</v>
+      </c>
       <c r="C241" s="1"/>
       <c r="D241" s="1"/>
     </row>
-    <row r="242" spans="3:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row r="242" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+      <c r="A242" s="23" t="s">
+        <v>447</v>
+      </c>
       <c r="C242" s="1"/>
       <c r="D242" s="1"/>
     </row>
-    <row r="243" spans="3:4" ht="35.5" x14ac:dyDescent="0.7">
-      <c r="C243" s="1"/>
-      <c r="D243" s="1"/>
-    </row>
-    <row r="244" spans="3:4" ht="35.5" x14ac:dyDescent="0.7">
-      <c r="C244" s="1"/>
-      <c r="D244" s="1"/>
+    <row r="243" spans="1:4" x14ac:dyDescent="0.65">
+      <c r="A243" s="23" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="244" spans="1:4" x14ac:dyDescent="0.65">
+      <c r="A244" s="23" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="245" spans="1:4" x14ac:dyDescent="0.65">
+      <c r="A245" s="23" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="246" spans="1:4" x14ac:dyDescent="0.65">
+      <c r="A246" s="23" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="247" spans="1:4" x14ac:dyDescent="0.65">
+      <c r="A247" s="24" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="248" spans="1:4" x14ac:dyDescent="0.65">
+      <c r="A248" s="23" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="249" spans="1:4" x14ac:dyDescent="0.65">
+      <c r="A249" s="23" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="250" spans="1:4" x14ac:dyDescent="0.65">
+      <c r="A250" s="23" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="251" spans="1:4" x14ac:dyDescent="0.65">
+      <c r="A251" s="23" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="252" spans="1:4" x14ac:dyDescent="0.65">
+      <c r="A252" s="23" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="253" spans="1:4" x14ac:dyDescent="0.65">
+      <c r="A253" s="23" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="254" spans="1:4" x14ac:dyDescent="0.65">
+      <c r="A254" s="23" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="255" spans="1:4" x14ac:dyDescent="0.65">
+      <c r="A255" s="23" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="256" spans="1:4" x14ac:dyDescent="0.65">
+      <c r="A256" s="23" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="257" spans="1:1" x14ac:dyDescent="0.65">
+      <c r="A257" s="23" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="258" spans="1:1" x14ac:dyDescent="0.65">
+      <c r="A258" s="23" t="s">
+        <v>453</v>
+      </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A202:B217">
-    <sortCondition ref="A202:A217"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A201:B215">
+    <sortCondition ref="A201:A215"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
@@ -4306,9 +4400,9 @@
     <hyperlink ref="B46" r:id="rId2" tooltip="View an OS map of this location on Bing Maps (new window)" display="https://www.bing.com/maps/default.aspx?setmkt=en-gb&amp;cp=52.750250345557~-4.0288421434674&amp;lvl=15&amp;style=s&amp;sp=point.52.750250345557_-4.0288421434674_Cerrig%20Arthur" xr:uid="{6854972D-F722-4473-8076-1406D591FB92}"/>
     <hyperlink ref="B77" r:id="rId3" tooltip="View an OS map of this location on Bing Maps (new window)" display="https://www.bing.com/maps/default.aspx?setmkt=en-gb&amp;cp=52.215454136212~-3.3260483997626&amp;lvl=15&amp;style=s&amp;sp=point.52.215454136212_-3.3260483997626_Gelli%20Hill%20Circle" xr:uid="{C8F5B7B6-ABAD-42F9-B507-C92A3183B978}"/>
     <hyperlink ref="B111" r:id="rId4" tooltip="View an OS map of this location on Bing Maps (new window)" display="https://www.bing.com/maps/default.aspx?setmkt=en-gb&amp;cp=52.591662305547~-3.6193494009883&amp;lvl=15&amp;style=s&amp;sp=point.52.591662305547_-3.6193494009883_Lled-Croen-Yr-Ych" xr:uid="{E961351D-516F-45CB-BF50-DD7B287FECB3}"/>
-    <hyperlink ref="B156" r:id="rId5" tooltip="View an OS map of this location on Bing Maps (new window)" display="https://www.bing.com/maps/default.aspx?setmkt=en-gb&amp;cp=52.212627380005~-3.2557091780359&amp;lvl=15&amp;style=s&amp;sp=point.52.212627380005_-3.2557091780359_Rhos-Maen" xr:uid="{93C8E83B-3BCF-4AB5-8AD8-B7F944463049}"/>
-    <hyperlink ref="B157" r:id="rId6" tooltip="View an OS map of this location on Bing Maps (new window)" display="https://www.bing.com/maps/default.aspx?setmkt=en-gb&amp;cp=52.861014281346~-3.4006087121138&amp;lvl=15&amp;style=s&amp;sp=point.52.861014281346_-3.4006087121138_Rhos%20Y%20Beddau%20%28Circle%29" xr:uid="{B7E779B5-4985-44AF-827E-3D43466B3F91}"/>
-    <hyperlink ref="B200" r:id="rId7" tooltip="View an OS map of this location on Bing Maps (new window)" display="https://www.bing.com/maps/default.aspx?setmkt=en-gb&amp;cp=52.5890125567~-3.47827442537&amp;lvl=15&amp;style=s&amp;sp=point.52.5890125567_-3.47827442537_Y%20Capel" xr:uid="{99B2A934-3A9F-46A6-BC82-DD305FF24EA6}"/>
+    <hyperlink ref="B155" r:id="rId5" tooltip="View an OS map of this location on Bing Maps (new window)" display="https://www.bing.com/maps/default.aspx?setmkt=en-gb&amp;cp=52.212627380005~-3.2557091780359&amp;lvl=15&amp;style=s&amp;sp=point.52.212627380005_-3.2557091780359_Rhos-Maen" xr:uid="{93C8E83B-3BCF-4AB5-8AD8-B7F944463049}"/>
+    <hyperlink ref="B156" r:id="rId6" tooltip="View an OS map of this location on Bing Maps (new window)" display="https://www.bing.com/maps/default.aspx?setmkt=en-gb&amp;cp=52.861014281346~-3.4006087121138&amp;lvl=15&amp;style=s&amp;sp=point.52.861014281346_-3.4006087121138_Rhos%20Y%20Beddau%20%28Circle%29" xr:uid="{B7E779B5-4985-44AF-827E-3D43466B3F91}"/>
+    <hyperlink ref="B199" r:id="rId7" tooltip="View an OS map of this location on Bing Maps (new window)" display="https://www.bing.com/maps/default.aspx?setmkt=en-gb&amp;cp=52.5890125567~-3.47827442537&amp;lvl=15&amp;style=s&amp;sp=point.52.5890125567_-3.47827442537_Y%20Capel" xr:uid="{99B2A934-3A9F-46A6-BC82-DD305FF24EA6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId8"/>

</xml_diff>

<commit_message>
Updated data with new sites supplied by dad. Added controls to exclude some columns.
</commit_message>
<xml_diff>
--- a/monument_classes/grid refs.xlsx
+++ b/monument_classes/grid refs.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="586" documentId="8_{A4E60168-C7DA-486C-8F65-DF4D7C1E74F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E1E1DA83-3CE1-4E82-815B-4C1C2AF7A867}"/>
   <bookViews>
-    <workbookView xWindow="-107" yWindow="-107" windowWidth="20847" windowHeight="11111" xr2:uid="{00C86CC1-D9DC-492E-B8C9-58A2E0E11513}"/>
+    <workbookView activeTab="0" windowHeight="11111" windowWidth="20847" xWindow="-107" xr2:uid="{00C86CC1-D9DC-492E-B8C9-58A2E0E11513}" yWindow="-107"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -767,10 +767,10 @@
     </r>
     <r>
       <rPr>
-        <sz val="28"/>
-        <color rgb="FFFF0000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <color rgb="FFFF0000"/>
+        <sz val="28"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
@@ -1425,117 +1425,155 @@
   </si>
   <si>
     <t>Shapbeck plantation</t>
+  </si>
+  <si>
+    <t>O o007727</t>
+  </si>
+  <si>
+    <t>O007727</t>
+  </si>
+  <si>
+    <t>Bektany</t>
+  </si>
+  <si>
+    <t>C254005</t>
+  </si>
+  <si>
+    <t>Boleycarrigeen</t>
+  </si>
+  <si>
+    <t>S935892</t>
+  </si>
+  <si>
+    <t>R695384</t>
+  </si>
+  <si>
+    <t>Ballynamona</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="17" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="8">
+    <numFmt numFmtId="5" formatCode="&quot;$&quot;#,##0_);(&quot;$&quot;#,##0)"/>
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red](&quot;$&quot;#,##0)"/>
+    <numFmt numFmtId="7" formatCode="&quot;$&quot;#,##0.00_);(&quot;$&quot;#,##0.00)"/>
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red](&quot;$&quot;#,##0.00)"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* (#,##0);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* (#,##0);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* (#,##0.00);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* (#,##0.00);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="17">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color rgb="FF000000"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color rgb="FF0563C1"/>
+      <sz val="11"/>
+      <u val="single"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color rgb="FF000000"/>
+      <sz val="8"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="26"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color rgb="FF000000"/>
+      <sz val="26"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="28"/>
-      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+      <color rgb="FF000000"/>
+      <sz val="28"/>
     </font>
     <font>
-      <sz val="28"/>
-      <color rgb="FF494948"/>
       <name val="Arial"/>
       <family val="2"/>
+      <color rgb="FF494948"/>
+      <sz val="28"/>
     </font>
     <font>
-      <sz val="28"/>
-      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <color rgb="FFFF0000"/>
+      <sz val="28"/>
     </font>
     <font>
-      <sz val="28"/>
       <name val="Arial"/>
       <family val="2"/>
+      <color rgb="FF000000"/>
+      <sz val="28"/>
     </font>
     <font>
-      <sz val="28"/>
-      <color rgb="FF424242"/>
       <name val="Arial"/>
       <family val="2"/>
+      <color rgb="FF424242"/>
+      <sz val="28"/>
     </font>
     <font>
-      <sz val="26"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color rgb="FF000000"/>
+      <sz val="26"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color rgb="FF000000"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="28"/>
-      <color rgb="FF424241"/>
       <name val="Arial"/>
       <family val="2"/>
+      <color rgb="FF424241"/>
+      <sz val="28"/>
     </font>
     <font>
-      <sz val="28"/>
-      <color rgb="FF040809"/>
       <name val="Arial"/>
       <family val="2"/>
+      <color rgb="FF040809"/>
+      <sz val="28"/>
     </font>
     <font>
-      <sz val="28"/>
-      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <color rgb="FF000000"/>
+      <sz val="28"/>
     </font>
     <font>
-      <sz val="36"/>
-      <color rgb="FF494948"/>
       <name val="Arial"/>
       <family val="2"/>
+      <color rgb="FF494948"/>
+      <sz val="36"/>
     </font>
     <font>
-      <sz val="28"/>
-      <color rgb="FF002020"/>
       <name val="Arial"/>
       <family val="2"/>
+      <color rgb="FF002020"/>
+      <sz val="28"/>
     </font>
     <font>
-      <sz val="28"/>
-      <color rgb="FF333333"/>
       <name val="Arial"/>
       <family val="2"/>
+      <color rgb="FF333333"/>
+      <sz val="28"/>
     </font>
   </fonts>
   <fills count="5">
@@ -1566,16 +1604,26 @@
   </fills>
   <borders count="1">
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal style="none">
+        <color rgb="FF000000"/>
+      </diagonal>
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellStyleXfs>
   <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1592,7 +1640,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1620,7 +1668,7 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1943,21 +1991,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6366B9E-07CC-4861-9D9F-9C4F681DA12F}">
-  <dimension ref="A1:E258"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6366B9E-07CC-4861-9D9F-9C4F681DA12F}">
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A204" workbookViewId="0">
-      <selection activeCell="A258" sqref="A258"/>
+    <sheetView topLeftCell="A204" workbookViewId="0" tabSelected="1">
+      <selection pane="topLeft" activeCell="A262" sqref="A262"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="34.950000000000003" x14ac:dyDescent="0.65"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="34"/>
   <cols>
     <col min="1" max="1" width="62.796875" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="32.5" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="1" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1965,13 +2012,13 @@
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
     </row>
-    <row r="2" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="2" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A2" s="3"/>
       <c r="B2" s="9"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="3" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A3" s="2" t="s">
         <v>241</v>
       </c>
@@ -1981,7 +2028,7 @@
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="4" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A4" s="2" t="s">
         <v>242</v>
       </c>
@@ -1991,7 +2038,7 @@
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="5" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A5" s="2" t="s">
         <v>244</v>
       </c>
@@ -2001,7 +2048,7 @@
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="6" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A6" s="2" t="s">
         <v>425</v>
       </c>
@@ -2011,7 +2058,7 @@
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="7" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A7" s="2" t="s">
         <v>426</v>
       </c>
@@ -2021,7 +2068,7 @@
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="8" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A8" s="2" t="s">
         <v>427</v>
       </c>
@@ -2031,7 +2078,7 @@
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
     </row>
-    <row r="9" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="9" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A9" s="2" t="s">
         <v>428</v>
       </c>
@@ -2041,7 +2088,7 @@
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="10" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A10" s="2" t="s">
         <v>1</v>
       </c>
@@ -2051,7 +2098,7 @@
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
     </row>
-    <row r="11" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="11" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A11" s="2" t="s">
         <v>2</v>
       </c>
@@ -2061,7 +2108,7 @@
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
     </row>
-    <row r="12" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="12" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A12" s="2" t="s">
         <v>3</v>
       </c>
@@ -2071,7 +2118,7 @@
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
     </row>
-    <row r="13" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="13" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A13" s="2" t="s">
         <v>4</v>
       </c>
@@ -2081,7 +2128,7 @@
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
     </row>
-    <row r="14" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="14" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A14" s="2" t="s">
         <v>246</v>
       </c>
@@ -2091,7 +2138,7 @@
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="15" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A15" s="2" t="s">
         <v>5</v>
       </c>
@@ -2101,7 +2148,7 @@
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="16" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A16" s="2" t="s">
         <v>248</v>
       </c>
@@ -2111,7 +2158,7 @@
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="17" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A17" s="2" t="s">
         <v>6</v>
       </c>
@@ -2121,7 +2168,7 @@
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="18" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A18" s="2" t="s">
         <v>7</v>
       </c>
@@ -2131,7 +2178,7 @@
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="19" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A19" s="2" t="s">
         <v>8</v>
       </c>
@@ -2141,7 +2188,7 @@
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="20" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A20" s="2" t="s">
         <v>9</v>
       </c>
@@ -2151,7 +2198,7 @@
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="21" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A21" s="2" t="s">
         <v>10</v>
       </c>
@@ -2161,7 +2208,7 @@
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="22" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A22" s="2" t="s">
         <v>11</v>
       </c>
@@ -2171,7 +2218,7 @@
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
     </row>
-    <row r="23" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="23" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A23" s="4" t="s">
         <v>12</v>
       </c>
@@ -2181,7 +2228,7 @@
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="24" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A24" s="2" t="s">
         <v>13</v>
       </c>
@@ -2191,7 +2238,7 @@
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="25" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A25" s="2" t="s">
         <v>14</v>
       </c>
@@ -2201,7 +2248,7 @@
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
     </row>
-    <row r="26" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="26" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A26" s="2" t="s">
         <v>15</v>
       </c>
@@ -2211,7 +2258,7 @@
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
     </row>
-    <row r="27" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="27" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A27" s="2" t="s">
         <v>16</v>
       </c>
@@ -2221,7 +2268,7 @@
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
     </row>
-    <row r="28" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="28" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A28" s="2" t="s">
         <v>17</v>
       </c>
@@ -2231,7 +2278,7 @@
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
     </row>
-    <row r="29" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="29" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A29" s="2" t="s">
         <v>18</v>
       </c>
@@ -2241,7 +2288,7 @@
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
     </row>
-    <row r="30" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="30" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A30" s="2" t="s">
         <v>224</v>
       </c>
@@ -2251,7 +2298,7 @@
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
     </row>
-    <row r="31" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="31" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A31" s="2" t="s">
         <v>19</v>
       </c>
@@ -2261,7 +2308,7 @@
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
     </row>
-    <row r="32" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="32" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A32" s="2" t="s">
         <v>20</v>
       </c>
@@ -2271,7 +2318,7 @@
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
     </row>
-    <row r="33" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="33" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A33" s="2" t="s">
         <v>21</v>
       </c>
@@ -2281,7 +2328,7 @@
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
     </row>
-    <row r="34" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="34" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A34" s="2" t="s">
         <v>22</v>
       </c>
@@ -2291,7 +2338,7 @@
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
     </row>
-    <row r="35" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="35" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A35" s="2" t="s">
         <v>23</v>
       </c>
@@ -2301,7 +2348,7 @@
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
     </row>
-    <row r="36" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="36" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A36" s="2" t="s">
         <v>24</v>
       </c>
@@ -2311,7 +2358,7 @@
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
     </row>
-    <row r="37" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="37" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A37" s="2" t="s">
         <v>25</v>
       </c>
@@ -2321,7 +2368,7 @@
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
     </row>
-    <row r="38" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="38" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A38" s="2" t="s">
         <v>262</v>
       </c>
@@ -2331,7 +2378,7 @@
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
     </row>
-    <row r="39" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="39" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A39" s="2" t="s">
         <v>26</v>
       </c>
@@ -2341,7 +2388,7 @@
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
     </row>
-    <row r="40" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="40" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A40" s="2" t="s">
         <v>27</v>
       </c>
@@ -2351,7 +2398,7 @@
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
     </row>
-    <row r="41" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="41" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A41" s="2" t="s">
         <v>185</v>
       </c>
@@ -2361,7 +2408,7 @@
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
     </row>
-    <row r="42" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="42" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A42" s="2" t="s">
         <v>28</v>
       </c>
@@ -2371,7 +2418,7 @@
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
     </row>
-    <row r="43" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="43" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A43" s="2" t="s">
         <v>29</v>
       </c>
@@ -2381,7 +2428,7 @@
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
     </row>
-    <row r="44" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="44" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A44" s="2" t="s">
         <v>30</v>
       </c>
@@ -2391,7 +2438,7 @@
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
     </row>
-    <row r="45" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="45" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A45" s="2" t="s">
         <v>31</v>
       </c>
@@ -2401,7 +2448,7 @@
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
     </row>
-    <row r="46" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="46" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A46" s="2" t="s">
         <v>32</v>
       </c>
@@ -2411,7 +2458,7 @@
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
     </row>
-    <row r="47" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="47" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A47" s="2" t="s">
         <v>33</v>
       </c>
@@ -2421,7 +2468,7 @@
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
     </row>
-    <row r="48" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="48" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A48" s="2" t="s">
         <v>34</v>
       </c>
@@ -2431,7 +2478,7 @@
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
     </row>
-    <row r="49" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="49" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A49" s="2" t="s">
         <v>35</v>
       </c>
@@ -2441,7 +2488,7 @@
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
     </row>
-    <row r="50" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="50" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A50" s="2" t="s">
         <v>36</v>
       </c>
@@ -2451,7 +2498,7 @@
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
     </row>
-    <row r="51" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="51" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A51" s="2" t="s">
         <v>434</v>
       </c>
@@ -2461,7 +2508,7 @@
       <c r="C51" s="1"/>
       <c r="D51" s="1"/>
     </row>
-    <row r="52" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="52" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A52" s="2" t="s">
         <v>37</v>
       </c>
@@ -2471,7 +2518,7 @@
       <c r="C52" s="1"/>
       <c r="D52" s="1"/>
     </row>
-    <row r="53" spans="1:4" s="15" customFormat="1" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="53" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.7">
       <c r="A53" s="9" t="s">
         <v>38</v>
       </c>
@@ -2481,7 +2528,7 @@
       <c r="C53" s="14"/>
       <c r="D53" s="14"/>
     </row>
-    <row r="54" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="54" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A54" s="2" t="s">
         <v>39</v>
       </c>
@@ -2491,7 +2538,7 @@
       <c r="C54" s="1"/>
       <c r="D54" s="1"/>
     </row>
-    <row r="55" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="55" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A55" s="2" t="s">
         <v>40</v>
       </c>
@@ -2501,7 +2548,7 @@
       <c r="C55" s="1"/>
       <c r="D55" s="1"/>
     </row>
-    <row r="56" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="56" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A56" s="2" t="s">
         <v>41</v>
       </c>
@@ -2511,7 +2558,7 @@
       <c r="C56" s="1"/>
       <c r="D56" s="1"/>
     </row>
-    <row r="57" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="57" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A57" s="2" t="s">
         <v>42</v>
       </c>
@@ -2521,7 +2568,7 @@
       <c r="C57" s="1"/>
       <c r="D57" s="1"/>
     </row>
-    <row r="58" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="58" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A58" s="2" t="s">
         <v>43</v>
       </c>
@@ -2531,7 +2578,7 @@
       <c r="C58" s="1"/>
       <c r="D58" s="1"/>
     </row>
-    <row r="59" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="59" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A59" s="2" t="s">
         <v>44</v>
       </c>
@@ -2541,7 +2588,7 @@
       <c r="C59" s="1"/>
       <c r="D59" s="1"/>
     </row>
-    <row r="60" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="60" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A60" s="2" t="s">
         <v>45</v>
       </c>
@@ -2551,7 +2598,7 @@
       <c r="C60" s="1"/>
       <c r="D60" s="1"/>
     </row>
-    <row r="61" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="61" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A61" s="2" t="s">
         <v>46</v>
       </c>
@@ -2561,7 +2608,7 @@
       <c r="C61" s="1"/>
       <c r="D61" s="1"/>
     </row>
-    <row r="62" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="62" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A62" s="2" t="s">
         <v>229</v>
       </c>
@@ -2571,7 +2618,7 @@
       <c r="C62" s="1"/>
       <c r="D62" s="1"/>
     </row>
-    <row r="63" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="63" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A63" s="4" t="s">
         <v>47</v>
       </c>
@@ -2583,7 +2630,7 @@
       </c>
       <c r="D63" s="1"/>
     </row>
-    <row r="64" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="64" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A64" s="2" t="s">
         <v>48</v>
       </c>
@@ -2593,7 +2640,7 @@
       <c r="C64" s="1"/>
       <c r="D64" s="1"/>
     </row>
-    <row r="65" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="65" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A65" s="2" t="s">
         <v>49</v>
       </c>
@@ -2603,7 +2650,7 @@
       <c r="C65" s="1"/>
       <c r="D65" s="1"/>
     </row>
-    <row r="66" spans="1:4" ht="44.6" x14ac:dyDescent="0.8">
+    <row ht="44.6" r="66" spans="1:4" x14ac:dyDescent="0.8">
       <c r="A66" s="2" t="s">
         <v>50</v>
       </c>
@@ -2613,7 +2660,7 @@
       <c r="C66" s="16"/>
       <c r="D66" s="1"/>
     </row>
-    <row r="67" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="67" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A67" s="2" t="s">
         <v>51</v>
       </c>
@@ -2623,7 +2670,7 @@
       <c r="C67" s="1"/>
       <c r="D67" s="1"/>
     </row>
-    <row r="68" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="68" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A68" s="2" t="s">
         <v>52</v>
       </c>
@@ -2633,7 +2680,7 @@
       <c r="C68" s="1"/>
       <c r="D68" s="1"/>
     </row>
-    <row r="69" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="69" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A69" s="2" t="s">
         <v>53</v>
       </c>
@@ -2643,7 +2690,7 @@
       <c r="C69" s="1"/>
       <c r="D69" s="1"/>
     </row>
-    <row r="70" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="70" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A70" s="2" t="s">
         <v>54</v>
       </c>
@@ -2653,7 +2700,7 @@
       <c r="C70" s="1"/>
       <c r="D70" s="1"/>
     </row>
-    <row r="71" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="71" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A71" s="2" t="s">
         <v>55</v>
       </c>
@@ -2663,7 +2710,7 @@
       <c r="C71" s="1"/>
       <c r="D71" s="1"/>
     </row>
-    <row r="72" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="72" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A72" s="2" t="s">
         <v>56</v>
       </c>
@@ -2673,7 +2720,7 @@
       <c r="C72" s="1"/>
       <c r="D72" s="1"/>
     </row>
-    <row r="73" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="73" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A73" s="2" t="s">
         <v>57</v>
       </c>
@@ -2683,7 +2730,7 @@
       <c r="C73" s="1"/>
       <c r="D73" s="1"/>
     </row>
-    <row r="74" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="74" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A74" s="2" t="s">
         <v>58</v>
       </c>
@@ -2693,7 +2740,7 @@
       <c r="C74" s="1"/>
       <c r="D74" s="1"/>
     </row>
-    <row r="75" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="75" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A75" s="2" t="s">
         <v>399</v>
       </c>
@@ -2703,7 +2750,7 @@
       <c r="C75" s="1"/>
       <c r="D75" s="1"/>
     </row>
-    <row r="76" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="76" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A76" s="2" t="s">
         <v>59</v>
       </c>
@@ -2713,7 +2760,7 @@
       <c r="C76" s="1"/>
       <c r="D76" s="1"/>
     </row>
-    <row r="77" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="77" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A77" s="2" t="s">
         <v>60</v>
       </c>
@@ -2723,7 +2770,7 @@
       <c r="C77" s="1"/>
       <c r="D77" s="1"/>
     </row>
-    <row r="78" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="78" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A78" s="2" t="s">
         <v>61</v>
       </c>
@@ -2733,7 +2780,7 @@
       <c r="C78" s="1"/>
       <c r="D78" s="1"/>
     </row>
-    <row r="79" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="79" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A79" s="2" t="s">
         <v>62</v>
       </c>
@@ -2743,7 +2790,7 @@
       <c r="C79" s="1"/>
       <c r="D79" s="1"/>
     </row>
-    <row r="80" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="80" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A80" s="2" t="s">
         <v>63</v>
       </c>
@@ -2753,7 +2800,7 @@
       <c r="C80" s="1"/>
       <c r="D80" s="1"/>
     </row>
-    <row r="81" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="81" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A81" s="2" t="s">
         <v>64</v>
       </c>
@@ -2763,7 +2810,7 @@
       <c r="C81" s="1"/>
       <c r="D81" s="1"/>
     </row>
-    <row r="82" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="82" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A82" s="2" t="s">
         <v>65</v>
       </c>
@@ -2773,7 +2820,7 @@
       <c r="C82" s="1"/>
       <c r="D82" s="1"/>
     </row>
-    <row r="83" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="83" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A83" s="2" t="s">
         <v>66</v>
       </c>
@@ -2783,7 +2830,7 @@
       <c r="C83" s="1"/>
       <c r="D83" s="1"/>
     </row>
-    <row r="84" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="84" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A84" s="2" t="s">
         <v>67</v>
       </c>
@@ -2793,7 +2840,7 @@
       <c r="C84" s="1"/>
       <c r="D84" s="1"/>
     </row>
-    <row r="85" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="85" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A85" s="2" t="s">
         <v>68</v>
       </c>
@@ -2803,7 +2850,7 @@
       <c r="C85" s="1"/>
       <c r="D85" s="1"/>
     </row>
-    <row r="86" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="86" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A86" s="2" t="s">
         <v>69</v>
       </c>
@@ -2813,7 +2860,7 @@
       <c r="C86" s="1"/>
       <c r="D86" s="1"/>
     </row>
-    <row r="87" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="87" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A87" s="2" t="s">
         <v>70</v>
       </c>
@@ -2823,7 +2870,7 @@
       <c r="C87" s="1"/>
       <c r="D87" s="1"/>
     </row>
-    <row r="88" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="88" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A88" s="2" t="s">
         <v>71</v>
       </c>
@@ -2833,7 +2880,7 @@
       <c r="C88" s="1"/>
       <c r="D88" s="1"/>
     </row>
-    <row r="89" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="89" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A89" s="2" t="s">
         <v>72</v>
       </c>
@@ -2843,7 +2890,7 @@
       <c r="C89" s="1"/>
       <c r="D89" s="1"/>
     </row>
-    <row r="90" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="90" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A90" s="2" t="s">
         <v>177</v>
       </c>
@@ -2853,7 +2900,7 @@
       <c r="C90" s="1"/>
       <c r="D90" s="1"/>
     </row>
-    <row r="91" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="91" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A91" s="2" t="s">
         <v>73</v>
       </c>
@@ -2863,7 +2910,7 @@
       <c r="C91" s="1"/>
       <c r="D91" s="1"/>
     </row>
-    <row r="92" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="92" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A92" s="2" t="s">
         <v>74</v>
       </c>
@@ -2873,7 +2920,7 @@
       <c r="C92" s="1"/>
       <c r="D92" s="1"/>
     </row>
-    <row r="93" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="93" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A93" s="2" t="s">
         <v>75</v>
       </c>
@@ -2883,7 +2930,7 @@
       <c r="C93" s="1"/>
       <c r="D93" s="1"/>
     </row>
-    <row r="94" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="94" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A94" s="2" t="s">
         <v>76</v>
       </c>
@@ -2893,7 +2940,7 @@
       <c r="C94" s="1"/>
       <c r="D94" s="1"/>
     </row>
-    <row r="95" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="95" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A95" s="2" t="s">
         <v>77</v>
       </c>
@@ -2903,7 +2950,7 @@
       <c r="C95" s="1"/>
       <c r="D95" s="1"/>
     </row>
-    <row r="96" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="96" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A96" s="2" t="s">
         <v>78</v>
       </c>
@@ -2913,7 +2960,7 @@
       <c r="C96" s="1"/>
       <c r="D96" s="1"/>
     </row>
-    <row r="97" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="97" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A97" s="2" t="s">
         <v>79</v>
       </c>
@@ -2923,7 +2970,7 @@
       <c r="C97" s="1"/>
       <c r="D97" s="1"/>
     </row>
-    <row r="98" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="98" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A98" s="2" t="s">
         <v>80</v>
       </c>
@@ -2933,7 +2980,7 @@
       <c r="C98" s="1"/>
       <c r="D98" s="1"/>
     </row>
-    <row r="99" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="99" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A99" s="2" t="s">
         <v>81</v>
       </c>
@@ -2943,7 +2990,7 @@
       <c r="C99" s="1"/>
       <c r="D99" s="1"/>
     </row>
-    <row r="100" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="100" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A100" s="2" t="s">
         <v>82</v>
       </c>
@@ -2953,7 +3000,7 @@
       <c r="C100" s="1"/>
       <c r="D100" s="1"/>
     </row>
-    <row r="101" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="101" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A101" s="2" t="s">
         <v>83</v>
       </c>
@@ -2963,7 +3010,7 @@
       <c r="C101" s="1"/>
       <c r="D101" s="1"/>
     </row>
-    <row r="102" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="102" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A102" s="2" t="s">
         <v>84</v>
       </c>
@@ -2973,7 +3020,7 @@
       <c r="C102" s="1"/>
       <c r="D102" s="1"/>
     </row>
-    <row r="103" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="103" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A103" s="2" t="s">
         <v>85</v>
       </c>
@@ -2983,7 +3030,7 @@
       <c r="C103" s="1"/>
       <c r="D103" s="1"/>
     </row>
-    <row r="104" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="104" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A104" s="2" t="s">
         <v>86</v>
       </c>
@@ -2993,7 +3040,7 @@
       <c r="C104" s="1"/>
       <c r="D104" s="1"/>
     </row>
-    <row r="105" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="105" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A105" s="2" t="s">
         <v>87</v>
       </c>
@@ -3003,7 +3050,7 @@
       <c r="C105" s="1"/>
       <c r="D105" s="1"/>
     </row>
-    <row r="106" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="106" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A106" s="2" t="s">
         <v>205</v>
       </c>
@@ -3013,7 +3060,7 @@
       <c r="C106" s="1"/>
       <c r="D106" s="1"/>
     </row>
-    <row r="107" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="107" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A107" s="2" t="s">
         <v>88</v>
       </c>
@@ -3023,7 +3070,7 @@
       <c r="C107" s="1"/>
       <c r="D107" s="1"/>
     </row>
-    <row r="108" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="108" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A108" s="2" t="s">
         <v>89</v>
       </c>
@@ -3033,7 +3080,7 @@
       <c r="C108" s="1"/>
       <c r="D108" s="1"/>
     </row>
-    <row r="109" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="109" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A109" s="2" t="s">
         <v>310</v>
       </c>
@@ -3043,7 +3090,7 @@
       <c r="C109" s="1"/>
       <c r="D109" s="1"/>
     </row>
-    <row r="110" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="110" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A110" s="2" t="s">
         <v>90</v>
       </c>
@@ -3053,7 +3100,7 @@
       <c r="C110" s="1"/>
       <c r="D110" s="1"/>
     </row>
-    <row r="111" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="111" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A111" s="2" t="s">
         <v>91</v>
       </c>
@@ -3063,7 +3110,7 @@
       <c r="C111" s="1"/>
       <c r="D111" s="1"/>
     </row>
-    <row r="112" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="112" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A112" s="2" t="s">
         <v>92</v>
       </c>
@@ -3073,7 +3120,7 @@
       <c r="C112" s="1"/>
       <c r="D112" s="1"/>
     </row>
-    <row r="113" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="113" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A113" s="2" t="s">
         <v>93</v>
       </c>
@@ -3083,7 +3130,7 @@
       <c r="C113" s="1"/>
       <c r="D113" s="1"/>
     </row>
-    <row r="114" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="114" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A114" s="2" t="s">
         <v>94</v>
       </c>
@@ -3093,7 +3140,7 @@
       <c r="C114" s="1"/>
       <c r="D114" s="1"/>
     </row>
-    <row r="115" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="115" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A115" s="2" t="s">
         <v>418</v>
       </c>
@@ -3103,7 +3150,7 @@
       <c r="C115" s="1"/>
       <c r="D115" s="1"/>
     </row>
-    <row r="116" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="116" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A116" s="2" t="s">
         <v>95</v>
       </c>
@@ -3113,7 +3160,7 @@
       <c r="C116" s="1"/>
       <c r="D116" s="1"/>
     </row>
-    <row r="117" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="117" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A117" s="2" t="s">
         <v>96</v>
       </c>
@@ -3123,7 +3170,7 @@
       <c r="C117" s="1"/>
       <c r="D117" s="1"/>
     </row>
-    <row r="118" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="118" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A118" s="2" t="s">
         <v>212</v>
       </c>
@@ -3133,7 +3180,7 @@
       <c r="C118" s="1"/>
       <c r="D118" s="1"/>
     </row>
-    <row r="119" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="119" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A119" s="2" t="s">
         <v>97</v>
       </c>
@@ -3143,7 +3190,7 @@
       <c r="C119" s="1"/>
       <c r="D119" s="1"/>
     </row>
-    <row r="120" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="120" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A120" s="2" t="s">
         <v>98</v>
       </c>
@@ -3153,7 +3200,7 @@
       <c r="C120" s="1"/>
       <c r="D120" s="1"/>
     </row>
-    <row r="121" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="121" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A121" s="2" t="s">
         <v>99</v>
       </c>
@@ -3163,7 +3210,7 @@
       <c r="C121" s="1"/>
       <c r="D121" s="1"/>
     </row>
-    <row r="122" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="122" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A122" s="2" t="s">
         <v>100</v>
       </c>
@@ -3173,7 +3220,7 @@
       <c r="C122" s="1"/>
       <c r="D122" s="1"/>
     </row>
-    <row r="123" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="123" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A123" s="2" t="s">
         <v>101</v>
       </c>
@@ -3183,7 +3230,7 @@
       <c r="C123" s="1"/>
       <c r="D123" s="1"/>
     </row>
-    <row r="124" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="124" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A124" s="2" t="s">
         <v>102</v>
       </c>
@@ -3193,7 +3240,7 @@
       <c r="C124" s="1"/>
       <c r="D124" s="1"/>
     </row>
-    <row r="125" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="125" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A125" s="2" t="s">
         <v>103</v>
       </c>
@@ -3203,7 +3250,7 @@
       <c r="C125" s="1"/>
       <c r="D125" s="1"/>
     </row>
-    <row r="126" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="126" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A126" s="2" t="s">
         <v>104</v>
       </c>
@@ -3213,7 +3260,7 @@
       <c r="C126" s="1"/>
       <c r="D126" s="1"/>
     </row>
-    <row r="127" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="127" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A127" s="2" t="s">
         <v>105</v>
       </c>
@@ -3223,7 +3270,7 @@
       <c r="C127" s="1"/>
       <c r="D127" s="1"/>
     </row>
-    <row r="128" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="128" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A128" s="2" t="s">
         <v>105</v>
       </c>
@@ -3233,7 +3280,7 @@
       <c r="C128" s="1"/>
       <c r="D128" s="1"/>
     </row>
-    <row r="129" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="129" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A129" s="2" t="s">
         <v>106</v>
       </c>
@@ -3243,7 +3290,7 @@
       <c r="C129" s="1"/>
       <c r="D129" s="1"/>
     </row>
-    <row r="130" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="130" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A130" s="2" t="s">
         <v>107</v>
       </c>
@@ -3253,7 +3300,7 @@
       <c r="C130" s="1"/>
       <c r="D130" s="1"/>
     </row>
-    <row r="131" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="131" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A131" s="2" t="s">
         <v>108</v>
       </c>
@@ -3263,7 +3310,7 @@
       <c r="C131" s="1"/>
       <c r="D131" s="1"/>
     </row>
-    <row r="132" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="132" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A132" s="2" t="s">
         <v>109</v>
       </c>
@@ -3273,7 +3320,7 @@
       <c r="C132" s="1"/>
       <c r="D132" s="1"/>
     </row>
-    <row r="133" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="133" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A133" s="2" t="s">
         <v>110</v>
       </c>
@@ -3283,7 +3330,7 @@
       <c r="C133" s="1"/>
       <c r="D133" s="1"/>
     </row>
-    <row r="134" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="134" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A134" s="4" t="s">
         <v>111</v>
       </c>
@@ -3293,7 +3340,7 @@
       <c r="C134" s="1"/>
       <c r="D134" s="1"/>
     </row>
-    <row r="135" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="135" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A135" s="2" t="s">
         <v>112</v>
       </c>
@@ -3303,7 +3350,7 @@
       <c r="C135" s="1"/>
       <c r="D135" s="1"/>
     </row>
-    <row r="136" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="136" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A136" s="2" t="s">
         <v>113</v>
       </c>
@@ -3313,7 +3360,7 @@
       <c r="C136" s="1"/>
       <c r="D136" s="1"/>
     </row>
-    <row r="137" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="137" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A137" s="2" t="s">
         <v>114</v>
       </c>
@@ -3323,7 +3370,7 @@
       <c r="C137" s="1"/>
       <c r="D137" s="1"/>
     </row>
-    <row r="138" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="138" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A138" s="2" t="s">
         <v>115</v>
       </c>
@@ -3333,7 +3380,7 @@
       <c r="C138" s="1"/>
       <c r="D138" s="1"/>
     </row>
-    <row r="139" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="139" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A139" s="2" t="s">
         <v>116</v>
       </c>
@@ -3343,7 +3390,7 @@
       <c r="C139" s="1"/>
       <c r="D139" s="1"/>
     </row>
-    <row r="140" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="140" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A140" s="2" t="s">
         <v>117</v>
       </c>
@@ -3353,7 +3400,7 @@
       <c r="C140" s="1"/>
       <c r="D140" s="1"/>
     </row>
-    <row r="141" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="141" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A141" s="2" t="s">
         <v>118</v>
       </c>
@@ -3363,7 +3410,7 @@
       <c r="C141" s="1"/>
       <c r="D141" s="1"/>
     </row>
-    <row r="142" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="142" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A142" s="2" t="s">
         <v>119</v>
       </c>
@@ -3373,7 +3420,7 @@
       <c r="C142" s="1"/>
       <c r="D142" s="1"/>
     </row>
-    <row r="143" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="143" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A143" s="2" t="s">
         <v>120</v>
       </c>
@@ -3383,7 +3430,7 @@
       <c r="C143" s="1"/>
       <c r="D143" s="1"/>
     </row>
-    <row r="144" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="144" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A144" s="2" t="s">
         <v>121</v>
       </c>
@@ -3393,7 +3440,7 @@
       <c r="C144" s="1"/>
       <c r="D144" s="1"/>
     </row>
-    <row r="145" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="145" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A145" s="2" t="s">
         <v>122</v>
       </c>
@@ -3403,7 +3450,7 @@
       <c r="C145" s="1"/>
       <c r="D145" s="1"/>
     </row>
-    <row r="146" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="146" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A146" s="2" t="s">
         <v>333</v>
       </c>
@@ -3413,7 +3460,7 @@
       <c r="C146" s="1"/>
       <c r="D146" s="1"/>
     </row>
-    <row r="147" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="147" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A147" s="2" t="s">
         <v>336</v>
       </c>
@@ -3423,7 +3470,7 @@
       <c r="C147" s="1"/>
       <c r="D147" s="1"/>
     </row>
-    <row r="148" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="148" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A148" s="2" t="s">
         <v>123</v>
       </c>
@@ -3433,7 +3480,7 @@
       <c r="C148" s="1"/>
       <c r="D148" s="1"/>
     </row>
-    <row r="149" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="149" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A149" s="2" t="s">
         <v>124</v>
       </c>
@@ -3443,7 +3490,7 @@
       <c r="C149" s="1"/>
       <c r="D149" s="1"/>
     </row>
-    <row r="150" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="150" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A150" s="2" t="s">
         <v>125</v>
       </c>
@@ -3453,7 +3500,7 @@
       <c r="C150" s="1"/>
       <c r="D150" s="1"/>
     </row>
-    <row r="151" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="151" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A151" s="2" t="s">
         <v>126</v>
       </c>
@@ -3463,7 +3510,7 @@
       <c r="C151" s="1"/>
       <c r="D151" s="1"/>
     </row>
-    <row r="152" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="152" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A152" s="2" t="s">
         <v>127</v>
       </c>
@@ -3473,7 +3520,7 @@
       <c r="C152" s="1"/>
       <c r="D152" s="1"/>
     </row>
-    <row r="153" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="153" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A153" s="2" t="s">
         <v>344</v>
       </c>
@@ -3483,7 +3530,7 @@
       <c r="C153" s="1"/>
       <c r="D153" s="1"/>
     </row>
-    <row r="154" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="154" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A154" s="2" t="s">
         <v>240</v>
       </c>
@@ -3493,7 +3540,7 @@
       <c r="C154" s="1"/>
       <c r="D154" s="1"/>
     </row>
-    <row r="155" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="155" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A155" s="2" t="s">
         <v>128</v>
       </c>
@@ -3503,7 +3550,7 @@
       <c r="C155" s="1"/>
       <c r="D155" s="1"/>
     </row>
-    <row r="156" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="156" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A156" s="2" t="s">
         <v>129</v>
       </c>
@@ -3513,7 +3560,7 @@
       <c r="C156" s="1"/>
       <c r="D156" s="1"/>
     </row>
-    <row r="157" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="157" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A157" s="2" t="s">
         <v>130</v>
       </c>
@@ -3523,7 +3570,7 @@
       <c r="C157" s="1"/>
       <c r="D157" s="1"/>
     </row>
-    <row r="158" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="158" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A158" s="2" t="s">
         <v>131</v>
       </c>
@@ -3533,7 +3580,7 @@
       <c r="C158" s="1"/>
       <c r="D158" s="1"/>
     </row>
-    <row r="159" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="159" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A159" s="2" t="s">
         <v>132</v>
       </c>
@@ -3543,7 +3590,7 @@
       <c r="C159" s="1"/>
       <c r="D159" s="1"/>
     </row>
-    <row r="160" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="160" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A160" s="2" t="s">
         <v>346</v>
       </c>
@@ -3553,7 +3600,7 @@
       <c r="C160" s="1"/>
       <c r="D160" s="1"/>
     </row>
-    <row r="161" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="161" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A161" s="2" t="s">
         <v>349</v>
       </c>
@@ -3563,7 +3610,7 @@
       <c r="C161" s="1"/>
       <c r="D161" s="1"/>
     </row>
-    <row r="162" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="162" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A162" s="2" t="s">
         <v>133</v>
       </c>
@@ -3573,7 +3620,7 @@
       <c r="C162" s="1"/>
       <c r="D162" s="1"/>
     </row>
-    <row r="163" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="163" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A163" s="2" t="s">
         <v>134</v>
       </c>
@@ -3583,7 +3630,7 @@
       <c r="C163" s="1"/>
       <c r="D163" s="1"/>
     </row>
-    <row r="164" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="164" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A164" s="2" t="s">
         <v>135</v>
       </c>
@@ -3593,7 +3640,7 @@
       <c r="C164" s="1"/>
       <c r="D164" s="1"/>
     </row>
-    <row r="165" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="165" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A165" s="2" t="s">
         <v>136</v>
       </c>
@@ -3603,7 +3650,7 @@
       <c r="C165" s="1"/>
       <c r="D165" s="1"/>
     </row>
-    <row r="166" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="166" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A166" s="2" t="s">
         <v>137</v>
       </c>
@@ -3613,7 +3660,7 @@
       <c r="C166" s="1"/>
       <c r="D166" s="1"/>
     </row>
-    <row r="167" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="167" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A167" s="2" t="s">
         <v>138</v>
       </c>
@@ -3623,7 +3670,7 @@
       <c r="C167" s="1"/>
       <c r="D167" s="1"/>
     </row>
-    <row r="168" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="168" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A168" s="2" t="s">
         <v>355</v>
       </c>
@@ -3633,7 +3680,7 @@
       <c r="C168" s="1"/>
       <c r="D168" s="1"/>
     </row>
-    <row r="169" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="169" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A169" s="2" t="s">
         <v>357</v>
       </c>
@@ -3643,7 +3690,7 @@
       <c r="C169" s="1"/>
       <c r="D169" s="1"/>
     </row>
-    <row r="170" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="170" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A170" s="2" t="s">
         <v>358</v>
       </c>
@@ -3653,7 +3700,7 @@
       <c r="C170" s="1"/>
       <c r="D170" s="1"/>
     </row>
-    <row r="171" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="171" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A171" s="2" t="s">
         <v>139</v>
       </c>
@@ -3663,7 +3710,7 @@
       <c r="C171" s="1"/>
       <c r="D171" s="1"/>
     </row>
-    <row r="172" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="172" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A172" s="2" t="s">
         <v>140</v>
       </c>
@@ -3673,7 +3720,7 @@
       <c r="C172" s="1"/>
       <c r="D172" s="1"/>
     </row>
-    <row r="173" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="173" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A173" s="2" t="s">
         <v>141</v>
       </c>
@@ -3683,7 +3730,7 @@
       <c r="C173" s="1"/>
       <c r="D173" s="1"/>
     </row>
-    <row r="174" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="174" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A174" s="2" t="s">
         <v>142</v>
       </c>
@@ -3693,7 +3740,7 @@
       <c r="C174" s="1"/>
       <c r="D174" s="1"/>
     </row>
-    <row r="175" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="175" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A175" s="2" t="s">
         <v>143</v>
       </c>
@@ -3703,7 +3750,7 @@
       <c r="C175" s="1"/>
       <c r="D175" s="1"/>
     </row>
-    <row r="176" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="176" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A176" s="2" t="s">
         <v>144</v>
       </c>
@@ -3713,7 +3760,7 @@
       <c r="C176" s="1"/>
       <c r="D176" s="1"/>
     </row>
-    <row r="177" spans="1:5" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="177" spans="1:5" x14ac:dyDescent="0.7">
       <c r="A177" s="2" t="s">
         <v>367</v>
       </c>
@@ -3723,7 +3770,7 @@
       <c r="C177" s="1"/>
       <c r="D177" s="1"/>
     </row>
-    <row r="178" spans="1:5" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="178" spans="1:5" x14ac:dyDescent="0.7">
       <c r="A178" s="2" t="s">
         <v>145</v>
       </c>
@@ -3733,7 +3780,7 @@
       <c r="C178" s="1"/>
       <c r="D178" s="1"/>
     </row>
-    <row r="179" spans="1:5" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="179" spans="1:5" x14ac:dyDescent="0.7">
       <c r="A179" s="2" t="s">
         <v>369</v>
       </c>
@@ -3743,7 +3790,7 @@
       <c r="C179" s="1"/>
       <c r="D179" s="1"/>
     </row>
-    <row r="180" spans="1:5" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="180" spans="1:5" x14ac:dyDescent="0.7">
       <c r="A180" s="2" t="s">
         <v>146</v>
       </c>
@@ -3753,7 +3800,7 @@
       <c r="C180" s="1"/>
       <c r="D180" s="1"/>
     </row>
-    <row r="181" spans="1:5" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="181" spans="1:5" x14ac:dyDescent="0.7">
       <c r="A181" s="2" t="s">
         <v>147</v>
       </c>
@@ -3763,7 +3810,7 @@
       <c r="C181" s="1"/>
       <c r="D181" s="1"/>
     </row>
-    <row r="182" spans="1:5" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="182" spans="1:5" x14ac:dyDescent="0.7">
       <c r="A182" s="2" t="s">
         <v>148</v>
       </c>
@@ -3773,7 +3820,7 @@
       <c r="C182" s="1"/>
       <c r="D182" s="1"/>
     </row>
-    <row r="183" spans="1:5" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="183" spans="1:5" x14ac:dyDescent="0.7">
       <c r="A183" s="2" t="s">
         <v>372</v>
       </c>
@@ -3783,7 +3830,7 @@
       <c r="C183" s="1"/>
       <c r="D183" s="1"/>
     </row>
-    <row r="184" spans="1:5" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="184" spans="1:5" x14ac:dyDescent="0.7">
       <c r="A184" s="2" t="s">
         <v>149</v>
       </c>
@@ -3793,7 +3840,7 @@
       <c r="C184" s="1"/>
       <c r="D184" s="1"/>
     </row>
-    <row r="185" spans="1:5" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="185" spans="1:5" x14ac:dyDescent="0.7">
       <c r="A185" s="2" t="s">
         <v>150</v>
       </c>
@@ -3803,7 +3850,7 @@
       <c r="C185" s="1"/>
       <c r="D185" s="1"/>
     </row>
-    <row r="186" spans="1:5" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="186" spans="1:5" x14ac:dyDescent="0.7">
       <c r="A186" s="2" t="s">
         <v>151</v>
       </c>
@@ -3813,7 +3860,7 @@
       <c r="C186" s="1"/>
       <c r="D186" s="1"/>
     </row>
-    <row r="187" spans="1:5" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="187" spans="1:5" x14ac:dyDescent="0.7">
       <c r="A187" s="2" t="s">
         <v>377</v>
       </c>
@@ -3822,11 +3869,8 @@
       </c>
       <c r="C187" s="1"/>
       <c r="D187" s="1"/>
-      <c r="E187">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="188" spans="1:5" ht="35.5" x14ac:dyDescent="0.7">
+    </row>
+    <row ht="35.5" r="188" spans="1:5" x14ac:dyDescent="0.7">
       <c r="A188" s="2" t="s">
         <v>152</v>
       </c>
@@ -3836,7 +3880,7 @@
       <c r="C188" s="1"/>
       <c r="D188" s="1"/>
     </row>
-    <row r="189" spans="1:5" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="189" spans="1:5" x14ac:dyDescent="0.7">
       <c r="A189" s="2" t="s">
         <v>153</v>
       </c>
@@ -3846,7 +3890,7 @@
       <c r="C189" s="1"/>
       <c r="D189" s="1"/>
     </row>
-    <row r="190" spans="1:5" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="190" spans="1:5" x14ac:dyDescent="0.7">
       <c r="A190" s="2" t="s">
         <v>154</v>
       </c>
@@ -3856,7 +3900,7 @@
       <c r="C190" s="1"/>
       <c r="D190" s="1"/>
     </row>
-    <row r="191" spans="1:5" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="191" spans="1:5" x14ac:dyDescent="0.7">
       <c r="A191" s="2" t="s">
         <v>155</v>
       </c>
@@ -3866,7 +3910,7 @@
       <c r="C191" s="1"/>
       <c r="D191" s="1"/>
     </row>
-    <row r="192" spans="1:5" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="192" spans="1:5" x14ac:dyDescent="0.7">
       <c r="A192" s="2" t="s">
         <v>156</v>
       </c>
@@ -3876,7 +3920,7 @@
       <c r="C192" s="1"/>
       <c r="D192" s="1"/>
     </row>
-    <row r="193" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="193" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A193" s="2" t="s">
         <v>157</v>
       </c>
@@ -3886,7 +3930,7 @@
       <c r="C193" s="1"/>
       <c r="D193" s="1"/>
     </row>
-    <row r="194" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="194" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A194" s="2" t="s">
         <v>158</v>
       </c>
@@ -3896,7 +3940,7 @@
       <c r="C194" s="1"/>
       <c r="D194" s="1"/>
     </row>
-    <row r="195" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="195" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A195" s="2" t="s">
         <v>159</v>
       </c>
@@ -3906,7 +3950,7 @@
       <c r="C195" s="1"/>
       <c r="D195" s="1"/>
     </row>
-    <row r="196" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="196" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A196" s="2" t="s">
         <v>160</v>
       </c>
@@ -3916,7 +3960,7 @@
       <c r="C196" s="1"/>
       <c r="D196" s="1"/>
     </row>
-    <row r="197" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="197" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A197" s="2" t="s">
         <v>161</v>
       </c>
@@ -3926,7 +3970,7 @@
       <c r="C197" s="1"/>
       <c r="D197" s="1"/>
     </row>
-    <row r="198" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="198" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A198" s="2" t="s">
         <v>162</v>
       </c>
@@ -3936,7 +3980,7 @@
       <c r="C198" s="1"/>
       <c r="D198" s="1"/>
     </row>
-    <row r="199" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="199" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A199" s="2" t="s">
         <v>163</v>
       </c>
@@ -3946,15 +3990,15 @@
       <c r="C199" s="1"/>
       <c r="D199" s="1"/>
     </row>
-    <row r="200" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="200" spans="1:4" x14ac:dyDescent="0.7">
       <c r="C200" s="1"/>
       <c r="D200" s="1"/>
     </row>
-    <row r="201" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="201" spans="1:4" x14ac:dyDescent="0.7">
       <c r="C201" s="1"/>
       <c r="D201" s="1"/>
     </row>
-    <row r="202" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="202" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A202" s="23" t="s">
         <v>340</v>
       </c>
@@ -3964,7 +4008,7 @@
       <c r="C202" s="1"/>
       <c r="D202" s="1"/>
     </row>
-    <row r="203" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="203" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A203" s="2" t="s">
         <v>207</v>
       </c>
@@ -3976,7 +4020,7 @@
       </c>
       <c r="D203" s="1"/>
     </row>
-    <row r="204" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="204" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A204" s="23" t="s">
         <v>186</v>
       </c>
@@ -3986,7 +4030,7 @@
       <c r="C204" s="1"/>
       <c r="D204" s="1"/>
     </row>
-    <row r="205" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="205" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A205" s="23" t="s">
         <v>164</v>
       </c>
@@ -3996,7 +4040,7 @@
       <c r="C205" s="1"/>
       <c r="D205" s="1"/>
     </row>
-    <row r="206" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="206" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A206" s="23" t="s">
         <v>173</v>
       </c>
@@ -4006,7 +4050,7 @@
       <c r="C206" s="1"/>
       <c r="D206" s="1"/>
     </row>
-    <row r="207" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="207" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A207" s="23" t="s">
         <v>385</v>
       </c>
@@ -4016,7 +4060,7 @@
       <c r="C207" s="1"/>
       <c r="D207" s="1"/>
     </row>
-    <row r="208" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="208" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A208" s="23" t="s">
         <v>205</v>
       </c>
@@ -4026,7 +4070,7 @@
       <c r="C208" s="1"/>
       <c r="D208" s="1"/>
     </row>
-    <row r="209" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="209" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A209" s="23" t="s">
         <v>179</v>
       </c>
@@ -4036,7 +4080,7 @@
       <c r="C209" s="1"/>
       <c r="D209" s="1"/>
     </row>
-    <row r="210" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="210" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A210" s="23" t="s">
         <v>386</v>
       </c>
@@ -4046,7 +4090,7 @@
       <c r="C210" s="1"/>
       <c r="D210" s="1"/>
     </row>
-    <row r="211" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="211" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A211" s="23" t="s">
         <v>455</v>
       </c>
@@ -4056,7 +4100,7 @@
       <c r="C211" s="1"/>
       <c r="D211" s="1"/>
     </row>
-    <row r="212" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="212" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A212" s="23" t="s">
         <v>392</v>
       </c>
@@ -4066,7 +4110,7 @@
       <c r="C212" s="1"/>
       <c r="D212" s="1"/>
     </row>
-    <row r="213" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="213" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A213" s="23" t="s">
         <v>395</v>
       </c>
@@ -4076,7 +4120,7 @@
       <c r="C213" s="1"/>
       <c r="D213" s="1"/>
     </row>
-    <row r="214" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="214" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A214" s="23" t="s">
         <v>403</v>
       </c>
@@ -4086,7 +4130,7 @@
       <c r="C214" s="1"/>
       <c r="D214" s="1"/>
     </row>
-    <row r="215" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="215" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A215" s="23" t="s">
         <v>183</v>
       </c>
@@ -4096,7 +4140,7 @@
       <c r="C215" s="1"/>
       <c r="D215" s="1"/>
     </row>
-    <row r="216" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="216" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A216" s="23" t="s">
         <v>406</v>
       </c>
@@ -4106,7 +4150,7 @@
       <c r="C216" s="1"/>
       <c r="D216" s="1"/>
     </row>
-    <row r="217" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="217" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A217" s="23" t="s">
         <v>393</v>
       </c>
@@ -4116,7 +4160,7 @@
       <c r="C217" s="1"/>
       <c r="D217" s="1"/>
     </row>
-    <row r="218" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="218" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A218" s="23" t="s">
         <v>195</v>
       </c>
@@ -4126,7 +4170,7 @@
       <c r="C218" s="1"/>
       <c r="D218" s="1"/>
     </row>
-    <row r="219" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="219" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A219" s="23" t="s">
         <v>413</v>
       </c>
@@ -4136,7 +4180,7 @@
       <c r="C219" s="1"/>
       <c r="D219" s="1"/>
     </row>
-    <row r="220" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="220" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A220" s="23" t="s">
         <v>414</v>
       </c>
@@ -4146,7 +4190,7 @@
       <c r="C220" s="1"/>
       <c r="D220" s="1"/>
     </row>
-    <row r="221" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="221" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A221" s="23" t="s">
         <v>415</v>
       </c>
@@ -4156,7 +4200,7 @@
       <c r="C221" s="2"/>
       <c r="D221" s="1"/>
     </row>
-    <row r="222" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="222" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A222" s="23" t="s">
         <v>421</v>
       </c>
@@ -4166,7 +4210,7 @@
       <c r="C222" s="1"/>
       <c r="D222" s="1"/>
     </row>
-    <row r="223" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="223" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A223" s="23" t="s">
         <v>419</v>
       </c>
@@ -4176,7 +4220,7 @@
       <c r="C223" s="1"/>
       <c r="D223" s="1"/>
     </row>
-    <row r="224" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="224" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A224" s="23" t="s">
         <v>420</v>
       </c>
@@ -4186,124 +4230,126 @@
       <c r="C224" s="1"/>
       <c r="D224" s="1"/>
     </row>
-    <row r="225" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="225" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A225" s="4" t="s">
         <v>437</v>
       </c>
-      <c r="B225" s="4"/>
+      <c r="B225" s="4" t="s">
+        <v>459</v>
+      </c>
       <c r="C225" s="1"/>
       <c r="D225" s="1"/>
     </row>
-    <row r="226" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="226" spans="1:4" x14ac:dyDescent="0.7">
       <c r="C226" s="1"/>
       <c r="D226" s="1"/>
     </row>
-    <row r="227" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="227" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A227" s="23" t="s">
         <v>438</v>
       </c>
       <c r="C227" s="1"/>
       <c r="D227" s="1"/>
     </row>
-    <row r="228" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="228" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A228" s="23" t="s">
         <v>439</v>
       </c>
       <c r="C228" s="1"/>
       <c r="D228" s="1"/>
     </row>
-    <row r="229" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="229" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A229" s="23" t="s">
         <v>440</v>
       </c>
       <c r="C229" s="1"/>
       <c r="D229" s="1"/>
     </row>
-    <row r="230" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="230" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A230" s="23" t="s">
         <v>441</v>
       </c>
       <c r="C230" s="1"/>
       <c r="D230" s="1"/>
     </row>
-    <row r="231" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="231" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A231" s="23" t="s">
         <v>442</v>
       </c>
       <c r="C231" s="1"/>
       <c r="D231" s="1"/>
     </row>
-    <row r="232" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="232" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A232" s="23" t="s">
         <v>393</v>
       </c>
       <c r="C232" s="1"/>
       <c r="D232" s="1"/>
     </row>
-    <row r="233" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="233" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A233" s="23" t="s">
         <v>456</v>
       </c>
       <c r="C233" s="1"/>
       <c r="D233" s="1"/>
     </row>
-    <row r="234" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="234" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A234" s="23" t="s">
         <v>443</v>
       </c>
       <c r="C234" s="1"/>
       <c r="D234" s="1"/>
     </row>
-    <row r="235" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="235" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A235" s="23" t="s">
         <v>444</v>
       </c>
       <c r="C235" s="1"/>
       <c r="D235" s="1"/>
     </row>
-    <row r="236" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="236" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A236" s="23" t="s">
         <v>229</v>
       </c>
       <c r="C236" s="1"/>
       <c r="D236" s="1"/>
     </row>
-    <row r="237" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="237" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A237" s="23" t="s">
         <v>399</v>
       </c>
       <c r="C237" s="1"/>
       <c r="D237" s="1"/>
     </row>
-    <row r="238" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="238" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A238" s="23" t="s">
         <v>415</v>
       </c>
       <c r="C238" s="1"/>
       <c r="D238" s="1"/>
     </row>
-    <row r="239" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="239" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A239" s="23" t="s">
         <v>445</v>
       </c>
       <c r="C239" s="1"/>
       <c r="D239" s="1"/>
     </row>
-    <row r="240" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="240" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A240" s="23" t="s">
         <v>310</v>
       </c>
       <c r="C240" s="1"/>
       <c r="D240" s="1"/>
     </row>
-    <row r="241" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="241" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A241" s="23" t="s">
         <v>446</v>
       </c>
       <c r="C241" s="1"/>
       <c r="D241" s="1"/>
     </row>
-    <row r="242" spans="1:4" ht="35.5" x14ac:dyDescent="0.7">
+    <row ht="35.5" r="242" spans="1:4" x14ac:dyDescent="0.7">
       <c r="A242" s="23" t="s">
         <v>447</v>
       </c>
@@ -4388,6 +4434,30 @@
     <row r="258" spans="1:1" x14ac:dyDescent="0.65">
       <c r="A258" s="23" t="s">
         <v>453</v>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259" s="2" t="s">
+        <v>460</v>
+      </c>
+      <c r="B259" s="2" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260" s="2" t="s">
+        <v>462</v>
+      </c>
+      <c r="B260" s="2" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" s="2" t="s">
+        <v>465</v>
+      </c>
+      <c r="B261" s="2" t="s">
+        <v>464</v>
       </c>
     </row>
   </sheetData>
@@ -4396,13 +4466,13 @@
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="B39" r:id="rId1" tooltip="View an OS map of this location on Bing Maps (new window)" display="https://www.bing.com/maps/default.aspx?setmkt=en-gb&amp;cp=52.176608138052~-3.8303359043637&amp;lvl=15&amp;style=s&amp;sp=point.52.176608138052_-3.8303359043637_Bryn%20y%20Gorlan" xr:uid="{A1E3756D-E28C-4718-82B1-9662B3168872}"/>
-    <hyperlink ref="B46" r:id="rId2" tooltip="View an OS map of this location on Bing Maps (new window)" display="https://www.bing.com/maps/default.aspx?setmkt=en-gb&amp;cp=52.750250345557~-4.0288421434674&amp;lvl=15&amp;style=s&amp;sp=point.52.750250345557_-4.0288421434674_Cerrig%20Arthur" xr:uid="{6854972D-F722-4473-8076-1406D591FB92}"/>
-    <hyperlink ref="B77" r:id="rId3" tooltip="View an OS map of this location on Bing Maps (new window)" display="https://www.bing.com/maps/default.aspx?setmkt=en-gb&amp;cp=52.215454136212~-3.3260483997626&amp;lvl=15&amp;style=s&amp;sp=point.52.215454136212_-3.3260483997626_Gelli%20Hill%20Circle" xr:uid="{C8F5B7B6-ABAD-42F9-B507-C92A3183B978}"/>
-    <hyperlink ref="B111" r:id="rId4" tooltip="View an OS map of this location on Bing Maps (new window)" display="https://www.bing.com/maps/default.aspx?setmkt=en-gb&amp;cp=52.591662305547~-3.6193494009883&amp;lvl=15&amp;style=s&amp;sp=point.52.591662305547_-3.6193494009883_Lled-Croen-Yr-Ych" xr:uid="{E961351D-516F-45CB-BF50-DD7B287FECB3}"/>
-    <hyperlink ref="B155" r:id="rId5" tooltip="View an OS map of this location on Bing Maps (new window)" display="https://www.bing.com/maps/default.aspx?setmkt=en-gb&amp;cp=52.212627380005~-3.2557091780359&amp;lvl=15&amp;style=s&amp;sp=point.52.212627380005_-3.2557091780359_Rhos-Maen" xr:uid="{93C8E83B-3BCF-4AB5-8AD8-B7F944463049}"/>
-    <hyperlink ref="B156" r:id="rId6" tooltip="View an OS map of this location on Bing Maps (new window)" display="https://www.bing.com/maps/default.aspx?setmkt=en-gb&amp;cp=52.861014281346~-3.4006087121138&amp;lvl=15&amp;style=s&amp;sp=point.52.861014281346_-3.4006087121138_Rhos%20Y%20Beddau%20%28Circle%29" xr:uid="{B7E779B5-4985-44AF-827E-3D43466B3F91}"/>
-    <hyperlink ref="B199" r:id="rId7" tooltip="View an OS map of this location on Bing Maps (new window)" display="https://www.bing.com/maps/default.aspx?setmkt=en-gb&amp;cp=52.5890125567~-3.47827442537&amp;lvl=15&amp;style=s&amp;sp=point.52.5890125567_-3.47827442537_Y%20Capel" xr:uid="{99B2A934-3A9F-46A6-BC82-DD305FF24EA6}"/>
+    <hyperlink ref="B39" r:id="rId1" display="https://www.bing.com/maps/default.aspx?setmkt=en-gb&amp;cp=52.176608138052~-3.8303359043637&amp;lvl=15&amp;style=s&amp;sp=point.52.176608138052_-3.8303359043637_Bryn%20y%20Gorlan" tooltip="View an OS map of this location on Bing Maps (new window)" xr:uid="{A1E3756D-E28C-4718-82B1-9662B3168872}"/>
+    <hyperlink ref="B46" r:id="rId2" display="https://www.bing.com/maps/default.aspx?setmkt=en-gb&amp;cp=52.750250345557~-4.0288421434674&amp;lvl=15&amp;style=s&amp;sp=point.52.750250345557_-4.0288421434674_Cerrig%20Arthur" tooltip="View an OS map of this location on Bing Maps (new window)" xr:uid="{6854972D-F722-4473-8076-1406D591FB92}"/>
+    <hyperlink ref="B77" r:id="rId3" display="https://www.bing.com/maps/default.aspx?setmkt=en-gb&amp;cp=52.215454136212~-3.3260483997626&amp;lvl=15&amp;style=s&amp;sp=point.52.215454136212_-3.3260483997626_Gelli%20Hill%20Circle" tooltip="View an OS map of this location on Bing Maps (new window)" xr:uid="{C8F5B7B6-ABAD-42F9-B507-C92A3183B978}"/>
+    <hyperlink ref="B111" r:id="rId4" display="https://www.bing.com/maps/default.aspx?setmkt=en-gb&amp;cp=52.591662305547~-3.6193494009883&amp;lvl=15&amp;style=s&amp;sp=point.52.591662305547_-3.6193494009883_Lled-Croen-Yr-Ych" tooltip="View an OS map of this location on Bing Maps (new window)" xr:uid="{E961351D-516F-45CB-BF50-DD7B287FECB3}"/>
+    <hyperlink ref="B155" r:id="rId5" display="https://www.bing.com/maps/default.aspx?setmkt=en-gb&amp;cp=52.212627380005~-3.2557091780359&amp;lvl=15&amp;style=s&amp;sp=point.52.212627380005_-3.2557091780359_Rhos-Maen" tooltip="View an OS map of this location on Bing Maps (new window)" xr:uid="{93C8E83B-3BCF-4AB5-8AD8-B7F944463049}"/>
+    <hyperlink ref="B156" r:id="rId6" display="https://www.bing.com/maps/default.aspx?setmkt=en-gb&amp;cp=52.861014281346~-3.4006087121138&amp;lvl=15&amp;style=s&amp;sp=point.52.861014281346_-3.4006087121138_Rhos%20Y%20Beddau%20%28Circle%29" tooltip="View an OS map of this location on Bing Maps (new window)" xr:uid="{B7E779B5-4985-44AF-827E-3D43466B3F91}"/>
+    <hyperlink ref="B199" r:id="rId7" display="https://www.bing.com/maps/default.aspx?setmkt=en-gb&amp;cp=52.5890125567~-3.47827442537&amp;lvl=15&amp;style=s&amp;sp=point.52.5890125567_-3.47827442537_Y%20Capel" tooltip="View an OS map of this location on Bing Maps (new window)" xr:uid="{99B2A934-3A9F-46A6-BC82-DD305FF24EA6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId8"/>

</xml_diff>